<commit_message>
Fix bug and remove excel parsing
</commit_message>
<xml_diff>
--- a/data/citizen-science-projects-nl.xlsx
+++ b/data/citizen-science-projects-nl.xlsx
@@ -792,7 +792,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>https://euring.org/dataandcodes/obtainingdata</t>
+          <t>https://euring.org/data-and-codes/obtaining-data</t>
         </is>
       </c>
     </row>
@@ -1128,7 +1128,7 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>https://www.globe.gov/globedata/visualizeandretrievedata</t>
+          <t>https://www.globe.gov/globe-data/visualize-and-retrieve-data</t>
         </is>
       </c>
     </row>
@@ -1190,7 +1190,7 @@
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>https://www.globe.gov/globedata/visualizeandretrievedata</t>
+          <t>https://www.globe.gov/globe-data/visualize-and-retrieve-data</t>
         </is>
       </c>
     </row>
@@ -2151,10 +2151,14 @@
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/bhic_repnot</t>
-        </is>
-      </c>
-      <c r="N30" t="inlineStr"/>
+          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/2/project/kha</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>https://www.wiewaswie.nl/</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2205,14 +2209,10 @@
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/2/project/kha</t>
-        </is>
-      </c>
-      <c r="N31" t="inlineStr">
-        <is>
-          <t>https://www.wiewaswie.nl/</t>
-        </is>
-      </c>
+          <t>https://velehanden.nl/projecten/bekijk/details/project/sahm_index_bevolkingsregisters</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2263,7 +2263,7 @@
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/project/sahm_index_bevolkingsregisters</t>
+          <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/wiewaswie_bvr</t>
         </is>
       </c>
       <c r="N32" t="inlineStr"/>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/wiewaswie_bvr</t>
+          <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/mai_tagging</t>
         </is>
       </c>
       <c r="N33" t="inlineStr"/>
@@ -2371,14 +2371,10 @@
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/picvh_zar</t>
-        </is>
-      </c>
-      <c r="N34" t="inlineStr">
-        <is>
-          <t>https://www.zeeuwsarchief.nl/zeeuwengezocht/</t>
-        </is>
-      </c>
+          <t>https://velehanden.nl/projecten/bekijk/details/page/2/status/closed/project/gda_2</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2429,10 +2425,14 @@
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/mai_tagging</t>
-        </is>
-      </c>
-      <c r="N35" t="inlineStr"/>
+          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/3/project/bhic_strafgevangenissen</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>http://www.bhic.nl/onderzoeken/hulp-bij-onderzoek/gevangenisarchieven</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2483,10 +2483,14 @@
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/page/2/status/closed/project/gda_2</t>
-        </is>
-      </c>
-      <c r="N36" t="inlineStr"/>
+          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/picvh_zar</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>https://www.zeeuwsarchief.nl/zeeuwen-gezocht/</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2537,12 +2541,12 @@
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/3/project/bhic_strafgevangenissen</t>
+          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/amsterdam_kaarten</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>http://www.bhic.nl/onderzoeken/hulpbijonderzoek/gevangenisarchieven</t>
+          <t>https://archief.amsterdam/inventarissen/details/10035</t>
         </is>
       </c>
     </row>
@@ -2595,12 +2599,12 @@
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/amsterdam_kaarten</t>
+          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/raa</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>https://archief.amsterdam/inventarissen/details/10035</t>
+          <t>https://www.regionaalarchiefalkmaar.nl/collecties/beelden/beelden-2/?q=kaarten&amp;mode=gallery&amp;view=horizontal</t>
         </is>
       </c>
     </row>
@@ -2653,14 +2657,10 @@
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/raa</t>
-        </is>
-      </c>
-      <c r="N39" t="inlineStr">
-        <is>
-          <t>https://www.regionaalarchiefalkmaar.nl/collecties/beelden/beelden2/?q=kaarten&amp;mode=gallery&amp;view=horizontal</t>
-        </is>
-      </c>
+          <t>https://velehanden.nl/projecten/bekijk/details/project/gra_tagging_vanderveen</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2711,7 +2711,7 @@
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/project/gra_tagging_vanderveen</t>
+          <t>https://velehanden.nl/projecten/bekijk/details/project/vua_train_kronieken_transkribus</t>
         </is>
       </c>
       <c r="N40" t="inlineStr"/>
@@ -2765,14 +2765,10 @@
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/2/project/picvh_han_nijmegen</t>
-        </is>
-      </c>
-      <c r="N41" t="inlineStr">
-        <is>
-          <t>https://studiezaal.nijmegen.nl/zoeken.php</t>
-        </is>
-      </c>
+          <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/bhic_repnot</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2823,12 +2819,12 @@
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/wfg_index</t>
+          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/2/project/picvh_han_nijmegen</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>https://www.westfriesarchief.nl/onderzoek/zoeken/personen</t>
+          <t>https://studiezaal.nijmegen.nl/zoeken.php</t>
         </is>
       </c>
     </row>
@@ -2881,10 +2877,14 @@
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/run_slavenregisters</t>
-        </is>
-      </c>
-      <c r="N43" t="inlineStr"/>
+          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/wfg_index</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>https://www.westfriesarchief.nl/onderzoek/zoeken/personen</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2935,14 +2935,10 @@
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/som_index</t>
-        </is>
-      </c>
-      <c r="N44" t="inlineStr">
-        <is>
-          <t>https://www.muziekschatten.nl/omroepmuziek#eyJ0eXBlIjoibGlzdCIsImF2YWlsYWJpbGl0eSI6W10sImNvbXBvc2VyIjpbXSwiY2F0ZWdvcnkiOltdLCJnZW5yZSI6W10sImNvbGxlY3Rpb24iOltdLCJpbnN0cnVtZW50IjpbXSwiZmFjZXRzIjp7ImF2YWlsYWJpbGl0eSI6eyJ0ZXJtcyI6eyJmaWVsZCI6ImF2YWlsYWJpbGl0eSIsInNpemUiOjEwMH19LCJjb21wb3NlciI6eyJ0ZXJtcyI6eyJmaWVsZCI6ImNvbXBvc2VyIiwic2l6ZSI6MTAwfX0sImNhdGVnb3J5Ijp7InRlcm1zIjp7ImZpZWxkIjoiY2F0ZWdvcnkiLCJzaXplIjoxMDB9fSwiZ2VucmUiOnsidGVybXMiOnsiZmllbGQiOiJnZW5yZSIsInNpemUiOjEwMH19LCJjb2xsZWN0aW9uIjp7InRlcm1zIjp7ImZpZWxkIjoiY29sbGVjdGlvbiIsInNpemUiOjEwMH19LCJ1bmRlZmluZWQiOnsidGVybXMiOnt9fX19</t>
-        </is>
-      </c>
+          <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/run_slavenregisters</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2993,12 +2989,12 @@
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/picvh_zar_index_terneuzenaxel</t>
+          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/som_index</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>https://www.zeeuwsarchief.nl/onderzoekhetzelf/</t>
+          <t>https://www.muziekschatten.nl/omroepmuziek#eyJ0eXBlIjoibGlzdCIsImF2YWlsYWJpbGl0eSI6W10sImNvbXBvc2VyIjpbXSwiY2F0ZWdvcnkiOltdLCJnZW5yZSI6W10sImNvbGxlY3Rpb24iOltdLCJpbnN0cnVtZW50IjpbXSwiZmFjZXRzIjp7ImF2YWlsYWJpbGl0eSI6eyJ0ZXJtcyI6eyJmaWVsZCI6ImF2YWlsYWJpbGl0eSIsInNpemUiOjEwMH19LCJjb21wb3NlciI6eyJ0ZXJtcyI6eyJmaWVsZCI6ImNvbXBvc2VyIiwic2l6ZSI6MTAwfX0sImNhdGVnb3J5Ijp7InRlcm1zIjp7ImZpZWxkIjoiY2F0ZWdvcnkiLCJzaXplIjoxMDB9fSwiZ2VucmUiOnsidGVybXMiOnsiZmllbGQiOiJnZW5yZSIsInNpemUiOjEwMH19LCJjb2xsZWN0aW9uIjp7InRlcm1zIjp7ImZpZWxkIjoiY29sbGVjdGlvbiIsInNpemUiOjEwMH19LCJ1bmRlZmluZWQiOnsidGVybXMiOnt9fX19</t>
         </is>
       </c>
     </row>
@@ -3051,10 +3047,14 @@
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/project/hga_index_gezinskaarten</t>
-        </is>
-      </c>
-      <c r="N46" t="inlineStr"/>
+          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/picvh_zar_index_terneuzenaxel</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>https://www.zeeuwsarchief.nl/onderzoek-het-zelf/</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -3168,7 +3168,7 @@
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>https://archief.amsterdam/uitleg/indexen/41pensioenkaarten18941915?utm_source=OpenArchieven&amp;utm_medium=browser&amp;utm_campaign=OpenData</t>
+          <t>https://archief.amsterdam/uitleg/indexen/41-pensioenkaarten-1894-1915?utm_source=OpenArchieven&amp;utm_medium=browser&amp;utm_campaign=OpenData</t>
         </is>
       </c>
     </row>
@@ -3387,14 +3387,10 @@
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/sahm_indexing_persons</t>
-        </is>
-      </c>
-      <c r="N52" t="inlineStr">
-        <is>
-          <t>https://www.samh.nl/</t>
-        </is>
-      </c>
+          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/picvh_run</t>
+        </is>
+      </c>
+      <c r="N52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -3445,10 +3441,14 @@
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/project/vua_train_kronieken_transkribus</t>
-        </is>
-      </c>
-      <c r="N53" t="inlineStr"/>
+          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/sahm_indexing_persons</t>
+        </is>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>https://www.samh.nl/</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -3670,7 +3670,7 @@
       </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t>https://archief.amsterdam/indexen/persons?f=%7B%22search_i_datum%22:%7B%22v%22:%5B%2218640000%22,%2218749999%22%5D,%22d%22:%221864%20%201874%22%7D%7D</t>
+          <t>https://archief.amsterdam/indexen/persons?f=%7B%22search_i_datum%22:%7B%22v%22:%5B%2218640000%22,%2218749999%22%5D,%22d%22:%221864%20-%201874%22%7D%7D</t>
         </is>
       </c>
     </row>
@@ -3728,7 +3728,7 @@
       </c>
       <c r="N58" t="inlineStr">
         <is>
-          <t>https://noordhollandsarchief.nl/beelden/beeldbank/?fq%5B%5D=search_s_afbeelding:%22Ja%22&amp;mode=gallery&amp;view=horizontal&amp;sort=random%7B1612191303970%7D%20asc</t>
+          <t>https://noord-hollandsarchief.nl/beelden/beeldbank/?fq%5B%5D=search_s_afbeelding:%22Ja%22&amp;mode=gallery&amp;view=horizontal&amp;sort=random%7B1612191303970%7D%20asc</t>
         </is>
       </c>
     </row>
@@ -3786,7 +3786,7 @@
       </c>
       <c r="N59" t="inlineStr">
         <is>
-          <t>https://www.kabk.nl/alumni/bachelorbeeldendekunst</t>
+          <t>https://www.kabk.nl/alumni/bachelor-beeldende-kunst</t>
         </is>
       </c>
     </row>
@@ -3898,7 +3898,7 @@
       </c>
       <c r="N61" t="inlineStr">
         <is>
-          <t>https://archief.amsterdam/indexen/persons?f=%7B%22search_i_datum%22:%7B%22v%22:%5B%2218740000%22,%2218939999%22%5D,%22d%22:%221874%20%201893%22%7D%7D</t>
+          <t>https://archief.amsterdam/indexen/persons?f=%7B%22search_i_datum%22:%7B%22v%22:%5B%2218740000%22,%2218939999%22%5D,%22d%22:%221874%20-%201893%22%7D%7D</t>
         </is>
       </c>
     </row>
@@ -4063,10 +4063,14 @@
       </c>
       <c r="M64" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/project/ja_ik_wil</t>
-        </is>
-      </c>
-      <c r="N64" t="inlineStr"/>
+          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/2/project/amsterdam_patient</t>
+        </is>
+      </c>
+      <c r="N64" t="inlineStr">
+        <is>
+          <t>https://archief.amsterdam/uitleg/indexen/42-patientenregisters-1818-1899?utm_source=OpenArchieven&amp;utm_medium=browser&amp;utm_campaign=OpenData</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -4175,7 +4179,7 @@
       </c>
       <c r="M66" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/picvh_run</t>
+          <t>https://velehanden.nl/projecten/bekijk/details/project/cbg_index_hal</t>
         </is>
       </c>
       <c r="N66" t="inlineStr"/>
@@ -4229,7 +4233,7 @@
       </c>
       <c r="M67" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/project/utrecht_transcription_notarieel</t>
+          <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/nfm_tagging_photos</t>
         </is>
       </c>
       <c r="N67" t="inlineStr"/>
@@ -4283,7 +4287,7 @@
       </c>
       <c r="M68" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/project/cbg_index_hal</t>
+          <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/leiden_na1</t>
         </is>
       </c>
       <c r="N68" t="inlineStr"/>
@@ -4337,10 +4341,14 @@
       </c>
       <c r="M69" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/nfm_tagging_photos</t>
-        </is>
-      </c>
-      <c r="N69" t="inlineStr"/>
+          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/3/project/militieregisters</t>
+        </is>
+      </c>
+      <c r="N69" t="inlineStr">
+        <is>
+          <t>https://www.openarch.nl/indexen/9/militieregisters?lang=nl</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -4391,10 +4399,14 @@
       </c>
       <c r="M70" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/leiden_na1</t>
-        </is>
-      </c>
-      <c r="N70" t="inlineStr"/>
+          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/amsterdam_vrije_volk</t>
+        </is>
+      </c>
+      <c r="N70" t="inlineStr">
+        <is>
+          <t>https://archief.amsterdam/beeldbank/?mode=gallery&amp;view=horizontal&amp;q=het%20vrije%20volk&amp;page=1&amp;reverse=0</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -4445,14 +4457,10 @@
       </c>
       <c r="M71" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/3/project/militieregisters</t>
-        </is>
-      </c>
-      <c r="N71" t="inlineStr">
-        <is>
-          <t>https://www.openarch.nl/indexen/9/militieregisters?lang=nl</t>
-        </is>
-      </c>
+          <t>https://velehanden.nl/projecten/bekijk/details/project/gda_index_huwelijk</t>
+        </is>
+      </c>
+      <c r="N71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -4503,12 +4511,12 @@
       </c>
       <c r="M72" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/amsterdam_vrije_volk</t>
+          <t>https://velehanden.nl/projecten/bekijk/details/project/brd_index_repertoria</t>
         </is>
       </c>
       <c r="N72" t="inlineStr">
         <is>
-          <t>https://archief.amsterdam/beeldbank/?mode=gallery&amp;view=horizontal&amp;q=het%20vrije%20volk&amp;page=1&amp;reverse=0</t>
+          <t>https://www.wiewaswie.nl/</t>
         </is>
       </c>
     </row>
@@ -4561,7 +4569,7 @@
       </c>
       <c r="M73" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/project/gda_index_huwelijk</t>
+          <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/frl</t>
         </is>
       </c>
       <c r="N73" t="inlineStr"/>
@@ -4615,14 +4623,10 @@
       </c>
       <c r="M74" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/project/brd_index_repertoria</t>
-        </is>
-      </c>
-      <c r="N74" t="inlineStr">
-        <is>
-          <t>https://www.wiewaswie.nl/</t>
-        </is>
-      </c>
+          <t>https://velehanden.nl/projecten/bekijk/details/project/vua_annoteer_kronieken_transkribus</t>
+        </is>
+      </c>
+      <c r="N74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -4673,10 +4677,14 @@
       </c>
       <c r="M75" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/frl</t>
-        </is>
-      </c>
-      <c r="N75" t="inlineStr"/>
+          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/3/project/nat_nbc</t>
+        </is>
+      </c>
+      <c r="N75" t="inlineStr">
+        <is>
+          <t>https://www.naturalis.nl/collectie</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -4727,14 +4735,10 @@
       </c>
       <c r="M76" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/3/project/nat_nbc</t>
-        </is>
-      </c>
-      <c r="N76" t="inlineStr">
-        <is>
-          <t>https://www.naturalis.nl/collectie</t>
-        </is>
-      </c>
+          <t>https://velehanden.nl/projecten/bekijk/details/page/2/status/closed/project/bhic_strafgevangenissen_2</t>
+        </is>
+      </c>
+      <c r="N76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -4785,7 +4789,7 @@
       </c>
       <c r="M77" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/page/2/status/closed/project/bhic_strafgevangenissen_2</t>
+          <t>https://velehanden.nl/projecten/bekijk/details/project/huy_correct_resoluties_transkribus</t>
         </is>
       </c>
       <c r="N77" t="inlineStr"/>
@@ -4839,10 +4843,14 @@
       </c>
       <c r="M78" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/project/huy_correct_resoluties_transkribus</t>
-        </is>
-      </c>
-      <c r="N78" t="inlineStr"/>
+          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/3/project/nijmegen_bvr</t>
+        </is>
+      </c>
+      <c r="N78" t="inlineStr">
+        <is>
+          <t>https://studiezaal.nijmegen.nl/zoeken.php?zoeken[beschrijvingsgroepen][2145654597]=2145654597</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -4893,14 +4901,10 @@
       </c>
       <c r="M79" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/3/project/nijmegen_bvr</t>
-        </is>
-      </c>
-      <c r="N79" t="inlineStr">
-        <is>
-          <t>https://studiezaal.nijmegen.nl/zoeken.php?zoeken[beschrijvingsgroepen][2145654597]=2145654597</t>
-        </is>
-      </c>
+          <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/picvh_bhic_bevolkingsregister</t>
+        </is>
+      </c>
+      <c r="N79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -4951,7 +4955,7 @@
       </c>
       <c r="M80" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/picvh_bhic_bevolkingsregister</t>
+          <t>https://velehanden.nl/projecten/bekijk/details/project/amsterdam_correct_notarieel_transkribus</t>
         </is>
       </c>
       <c r="N80" t="inlineStr"/>
@@ -5005,7 +5009,7 @@
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/project/amsterdam_correct_notarieel_transkribus</t>
+          <t>https://velehanden.nl/projecten/bekijk/details/project/hga_index_gezinskaarten</t>
         </is>
       </c>
       <c r="N81" t="inlineStr"/>
@@ -5229,7 +5233,7 @@
       </c>
       <c r="M85" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/project/hfl_tagging_rijpcollectie</t>
+          <t>https://velehanden.nl/projecten/bekijk/details/project/ja_ik_wil</t>
         </is>
       </c>
       <c r="N85" t="inlineStr"/>
@@ -5283,14 +5287,10 @@
       </c>
       <c r="M86" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/2/project/amsterdam_patient</t>
-        </is>
-      </c>
-      <c r="N86" t="inlineStr">
-        <is>
-          <t>https://archief.amsterdam/uitleg/indexen/42patientenregisters18181899?utm_source=OpenArchieven&amp;utm_medium=browser&amp;utm_campaign=OpenData</t>
-        </is>
-      </c>
+          <t>https://velehanden.nl/projecten/bekijk/details/project/hfl_tagging_rijpcollectie</t>
+        </is>
+      </c>
+      <c r="N86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -5346,7 +5346,7 @@
       </c>
       <c r="N87" t="inlineStr">
         <is>
-          <t>https://archief.amsterdam/uitleg/indexen/65bevolkingsregisterovergenomendelen18921920?utm_source=OpenArchieven&amp;utm_medium=browser&amp;utm_campaign=OpenData</t>
+          <t>https://archief.amsterdam/uitleg/indexen/65-bevolkingsregister-overgenomen-delen-1892-1920?utm_source=OpenArchieven&amp;utm_medium=browser&amp;utm_campaign=OpenData</t>
         </is>
       </c>
     </row>
@@ -5399,10 +5399,14 @@
       </c>
       <c r="M88" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/project/vua_annoteer_kronieken_transkribus</t>
-        </is>
-      </c>
-      <c r="N88" t="inlineStr"/>
+          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/2/project/picvh_han</t>
+        </is>
+      </c>
+      <c r="N88" t="inlineStr">
+        <is>
+          <t>https://www.huisvandenijmeegsegeschiedenis.nl/info/Deelnemersregistratie_Vierdaagse</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -5453,12 +5457,12 @@
       </c>
       <c r="M89" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/2/project/picvh_han</t>
+          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/dre_index_inschrijvingsregisters</t>
         </is>
       </c>
       <c r="N89" t="inlineStr">
         <is>
-          <t>https://www.huisvandenijmeegsegeschiedenis.nl/info/Deelnemersregistratie_Vierdaagse</t>
+          <t>https://www.drentsarchief.nl/onderzoeken/zoektips/stamboomonderzoek</t>
         </is>
       </c>
     </row>
@@ -5511,14 +5515,10 @@
       </c>
       <c r="M90" t="inlineStr">
         <is>
-          <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/dre_index_inschrijvingsregisters</t>
-        </is>
-      </c>
-      <c r="N90" t="inlineStr">
-        <is>
-          <t>https://www.drentsarchief.nl/onderzoeken/zoektips/stamboomonderzoek</t>
-        </is>
-      </c>
+          <t>https://velehanden.nl/projecten/bekijk/details/project/utrecht_transcription_notarieel</t>
+        </is>
+      </c>
+      <c r="N90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -5896,7 +5896,7 @@
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>https://archief.amsterdam/uitleg/indexen/67bevolkingsregistergeannexeerdegemeenten18301921</t>
+          <t>https://archief.amsterdam/uitleg/indexen/67-bevolkingsregister-geannexeerde-gemeenten-1830-1921</t>
         </is>
       </c>
     </row>
@@ -6398,7 +6398,7 @@
       </c>
       <c r="N106" t="inlineStr">
         <is>
-          <t>https://hetutrechtsarchief.nl/onderzoek/resultaten/archieven?mivast=39&amp;mizig=210&amp;miadt=39&amp;miaet=1&amp;micode=10072&amp;minr=1307084&amp;miview=inv2&amp;milang=nl</t>
+          <t>https://hetutrechtsarchief.nl/onderzoek/resultaten/archieven?mivast=39&amp;mizig=210&amp;miadt=39&amp;miaet=1&amp;micode=1007-2&amp;minr=1307084&amp;miview=inv2&amp;milang=nl</t>
         </is>
       </c>
     </row>
@@ -6734,7 +6734,7 @@
       </c>
       <c r="N112" t="inlineStr">
         <is>
-          <t>https://stadsarchief.breda.nl/collectie/archief/genealogischebronnen/persons</t>
+          <t>https://stadsarchief.breda.nl/collectie/archief/genealogische-bronnen/persons</t>
         </is>
       </c>
     </row>
@@ -7074,7 +7074,7 @@
       </c>
       <c r="N118" t="inlineStr">
         <is>
-          <t>https://erfgoedcentrumzutphen.nl/onderzoeken/archieven/details/NLZuRAZ0110/path/2.4.1.2.19</t>
+          <t>https://erfgoedcentrumzutphen.nl/onderzoeken/archieven/details/NL-ZuRAZ-0110/path/2.4.1.2.19</t>
         </is>
       </c>
     </row>
@@ -7190,7 +7190,7 @@
       </c>
       <c r="N120" t="inlineStr">
         <is>
-          <t>https://login.munisense.net/login?url=https%3A%2F%2Foutdoorclimate.munisense.net%2F&amp;theme=munisensev2lhis</t>
+          <t>https://login.munisense.net/login?url=https%3A%2F%2Foutdoorclimate.munisense.net%2F&amp;theme=munisense-v2-lhis</t>
         </is>
       </c>
     </row>
@@ -7492,7 +7492,7 @@
       </c>
       <c r="N125" t="inlineStr">
         <is>
-          <t>https://www.tudelft.nl/scd/waterlab/doemeeaanonderzoek/onderzoeksresultaten</t>
+          <t>https://www.tudelft.nl/scd/waterlab/doe-mee-aan-onderzoek/onderzoeksresultaten</t>
         </is>
       </c>
     </row>
@@ -7612,7 +7612,7 @@
       </c>
       <c r="N127" t="inlineStr">
         <is>
-          <t>https://milieudefensie.nl/actueel/rapportwatademjijin.pdf</t>
+          <t>https://milieudefensie.nl/actueel/rapport-wat-adem-jij-in.pdf</t>
         </is>
       </c>
     </row>
@@ -7852,7 +7852,7 @@
       </c>
       <c r="N131" t="inlineStr">
         <is>
-          <t>https://grafana.sensemakersams.org/d/m2HAkciWk/mijnomgeving?orgId=1</t>
+          <t>https://grafana.sensemakersams.org/d/m2HAkciWk/mijn-omgeving?orgId=1</t>
         </is>
       </c>
     </row>
@@ -8439,14 +8439,10 @@
       </c>
       <c r="M141" t="inlineStr">
         <is>
-          <t>https://www.samenmetenaanluchtkwaliteit.nl/burgermetingen-schiedam</t>
-        </is>
-      </c>
-      <c r="N141" t="inlineStr">
-        <is>
-          <t>https://www.webgispublisher.nl/schiedam/</t>
-        </is>
-      </c>
+          <t>https://www.tudelft.nl/scd/waterlab/doe-mee-aan-onderzoek/project-5-zet-m-op-70</t>
+        </is>
+      </c>
+      <c r="N141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -8501,10 +8497,14 @@
       </c>
       <c r="M142" t="inlineStr">
         <is>
-          <t>https://www.tudelft.nl/scd/waterlab/doe-mee-aan-onderzoek/project-5-zet-m-op-70</t>
-        </is>
-      </c>
-      <c r="N142" t="inlineStr"/>
+          <t>https://hollandseluchten.waag.org/</t>
+        </is>
+      </c>
+      <c r="N142" t="inlineStr">
+        <is>
+          <t>https://hollandseluchten.waag.org/kaart/</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -8559,12 +8559,12 @@
       </c>
       <c r="M143" t="inlineStr">
         <is>
-          <t>https://hollandseluchten.waag.org/</t>
+          <t>https://drinkablerivers.org/what-we-do/citizen-science/</t>
         </is>
       </c>
       <c r="N143" t="inlineStr">
         <is>
-          <t>https://hollandseluchten.waag.org/kaart/</t>
+          <t>https://www.tudelft.nl/scd/waterlab/doe-mee-aan-onderzoek/onderzoeksresultaten</t>
         </is>
       </c>
     </row>
@@ -8617,14 +8617,10 @@
       </c>
       <c r="M144" t="inlineStr">
         <is>
-          <t>https://drinkablerivers.org/what-we-do/citizen-science/</t>
-        </is>
-      </c>
-      <c r="N144" t="inlineStr">
-        <is>
-          <t>https://www.tudelft.nl/scd/waterlab/doemeeaanonderzoek/onderzoeksresultaten</t>
-        </is>
-      </c>
+          <t>https://globenederland.nl/onderzoeksprojecten/lichtmeting/</t>
+        </is>
+      </c>
+      <c r="N144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -8675,7 +8671,7 @@
       </c>
       <c r="M145" t="inlineStr">
         <is>
-          <t>https://globenederland.nl/onderzoeksprojecten/lichtmeting/</t>
+          <t>https://www.scorewater.eu/#3cases</t>
         </is>
       </c>
       <c r="N145" t="inlineStr"/>
@@ -8733,10 +8729,14 @@
       </c>
       <c r="M146" t="inlineStr">
         <is>
-          <t>https://www.scorewater.eu/#3cases</t>
-        </is>
-      </c>
-      <c r="N146" t="inlineStr"/>
+          <t>https://www.samenmetenaanluchtkwaliteit.nl/snuffelfiets</t>
+        </is>
+      </c>
+      <c r="N146" t="inlineStr">
+        <is>
+          <t>https://snuffelfiets.nl/data/</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -8795,12 +8795,12 @@
       </c>
       <c r="M147" t="inlineStr">
         <is>
-          <t>https://www.samenmetenaanluchtkwaliteit.nl/snuffelfiets</t>
+          <t>https://www.eyeonwater.org/about-us</t>
         </is>
       </c>
       <c r="N147" t="inlineStr">
         <is>
-          <t>https://snuffelfiets.nl/data/</t>
+          <t>https://www.eyeonwater.org/search/</t>
         </is>
       </c>
     </row>
@@ -8857,12 +8857,12 @@
       </c>
       <c r="M148" t="inlineStr">
         <is>
-          <t>https://www.eyeonwater.org/about-us</t>
+          <t>https://amsterdamsounds.waag.org/</t>
         </is>
       </c>
       <c r="N148" t="inlineStr">
         <is>
-          <t>https://www.eyeonwater.org/search/</t>
+          <t>https://amsterdamsounds.waag.org/kaart/</t>
         </is>
       </c>
     </row>
@@ -8919,12 +8919,12 @@
       </c>
       <c r="M149" t="inlineStr">
         <is>
-          <t>https://amsterdamsounds.waag.org/</t>
+          <t>https://explane.org/#:~:text=ExPlane%20is%20the%20app%20to%20register%20aviation%20noise&amp;text=The%20app%20gives%20you%20the,by%20residents%20living%20near%20airports</t>
         </is>
       </c>
       <c r="N149" t="inlineStr">
         <is>
-          <t>https://amsterdamsounds.waag.org/kaart/</t>
+          <t>https://reports.explane.org/nl/</t>
         </is>
       </c>
     </row>
@@ -8977,14 +8977,10 @@
       </c>
       <c r="M150" t="inlineStr">
         <is>
-          <t>https://explane.org/#:~:text=ExPlane%20is%20the%20app%20to%20register%20aviation%20noise&amp;text=The%20app%20gives%20you%20the,by%20residents%20living%20near%20airports</t>
-        </is>
-      </c>
-      <c r="N150" t="inlineStr">
-        <is>
-          <t>https://reports.explane.org/nl/</t>
-        </is>
-      </c>
+          <t>https://www.tudelft.nl/scd/waterlab/doe-mee-aan-onderzoek/project-2-check-de-stadsvergroening</t>
+        </is>
+      </c>
+      <c r="N150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -9035,10 +9031,14 @@
       </c>
       <c r="M151" t="inlineStr">
         <is>
-          <t>https://www.tudelft.nl/scd/waterlab/doe-mee-aan-onderzoek/project-2-check-de-stadsvergroening</t>
-        </is>
-      </c>
-      <c r="N151" t="inlineStr"/>
+          <t>https://www.samenmetenaanluchtkwaliteit.nl/projecten/samen-luchtkwaliteit-meten-in-zuid-holland</t>
+        </is>
+      </c>
+      <c r="N151" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://samenmeten.rivm.nl/dataportaal/  </t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -9093,12 +9093,12 @@
       </c>
       <c r="M152" t="inlineStr">
         <is>
-          <t>https://www.samenmetenaanluchtkwaliteit.nl/projecten/samen-luchtkwaliteit-meten-in-zuid-holland</t>
+          <t xml:space="preserve">https://www.samenmetenaanluchtkwaliteit.nl/projecten/samen-houtrook-meten </t>
         </is>
       </c>
       <c r="N152" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://samenmeten.rivm.nl/dataportaal/  </t>
+          <t>https://samenmeten.rivm.nl/dataportaal/</t>
         </is>
       </c>
     </row>
@@ -9159,7 +9159,7 @@
       </c>
       <c r="M153" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://www.samenmetenaanluchtkwaliteit.nl/projecten/samen-houtrook-meten </t>
+          <t>https://www.samenmetenaanluchtkwaliteit.nl/vuurwerkexperiment-2018-2019</t>
         </is>
       </c>
       <c r="N153" t="inlineStr">
@@ -9217,12 +9217,12 @@
       </c>
       <c r="M154" t="inlineStr">
         <is>
-          <t>https://www.samenmetenaanluchtkwaliteit.nl/vuurwerkexperiment-2018-2019</t>
+          <t>https://almeremeetwater.nl/</t>
         </is>
       </c>
       <c r="N154" t="inlineStr">
         <is>
-          <t>https://samenmeten.rivm.nl/dataportaal/</t>
+          <t>https://almeremeetwater.nl/kaart/</t>
         </is>
       </c>
     </row>
@@ -9279,12 +9279,12 @@
       </c>
       <c r="M155" t="inlineStr">
         <is>
-          <t>https://almeremeetwater.nl/</t>
+          <t>https://www.tudelft.nl/scd/waterlab/doe-mee-aan-onderzoek/project-1-waterkwaliteit-in-europa</t>
         </is>
       </c>
       <c r="N155" t="inlineStr">
         <is>
-          <t>https://almeremeetwater.nl/kaart/</t>
+          <t>https://www.arcgis.com/home/webmap/viewer.html?webmap=9f6c2e258f2f40a884335feaf85501a7&amp;extent=3.9538,51.8158,4.968,52.1811</t>
         </is>
       </c>
     </row>
@@ -9337,12 +9337,12 @@
       </c>
       <c r="M156" t="inlineStr">
         <is>
-          <t>https://www.tudelft.nl/scd/waterlab/doe-mee-aan-onderzoek/project-1-waterkwaliteit-in-europa</t>
+          <t>https://data.smartemission.nl/home</t>
         </is>
       </c>
       <c r="N156" t="inlineStr">
         <is>
-          <t>https://www.arcgis.com/home/webmap/viewer.html?webmap=9f6c2e258f2f40a884335feaf85501a7&amp;extent=3.9538,51.8158,4.968,52.1811</t>
+          <t>https://data.smartemission.nl/data</t>
         </is>
       </c>
     </row>
@@ -9399,12 +9399,12 @@
       </c>
       <c r="M157" t="inlineStr">
         <is>
-          <t>https://data.smartemission.nl/home</t>
+          <t>https://www.meetjestad.net/nl/MeetjeStad</t>
         </is>
       </c>
       <c r="N157" t="inlineStr">
         <is>
-          <t>https://data.smartemission.nl/data</t>
+          <t>https://www.meetjestad.net/data/</t>
         </is>
       </c>
     </row>
@@ -9461,12 +9461,12 @@
       </c>
       <c r="M158" t="inlineStr">
         <is>
-          <t>https://www.meetjestad.net/nl/MeetjeStad</t>
+          <t>https://www.samenmetenaanluchtkwaliteit.nl/vuurwerkexperiment-20172018</t>
         </is>
       </c>
       <c r="N158" t="inlineStr">
         <is>
-          <t>https://www.meetjestad.net/data/</t>
+          <t>https://samenmeten.rivm.nl/dataportaal/</t>
         </is>
       </c>
     </row>
@@ -9519,14 +9519,10 @@
       </c>
       <c r="M159" t="inlineStr">
         <is>
-          <t>https://www.samenmetenaanluchtkwaliteit.nl/vuurwerkexperiment-20172018</t>
-        </is>
-      </c>
-      <c r="N159" t="inlineStr">
-        <is>
-          <t>https://samenmeten.rivm.nl/dataportaal/</t>
-        </is>
-      </c>
+          <t>https://www.samenmetenaanluchtkwaliteit.nl/ispex</t>
+        </is>
+      </c>
+      <c r="N159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -9577,7 +9573,7 @@
       </c>
       <c r="M160" t="inlineStr">
         <is>
-          <t>https://www.samenmetenaanluchtkwaliteit.nl/ispex</t>
+          <t>https://www.samenmetenaanluchtkwaliteit.nl/aireas-eindhoven</t>
         </is>
       </c>
       <c r="N160" t="inlineStr"/>
@@ -9635,10 +9631,14 @@
       </c>
       <c r="M161" t="inlineStr">
         <is>
-          <t>https://www.samenmetenaanluchtkwaliteit.nl/aireas-eindhoven</t>
-        </is>
-      </c>
-      <c r="N161" t="inlineStr"/>
+          <t>https://www.samenmetenaanluchtkwaliteit.nl/oud-nieuw-2020-2021</t>
+        </is>
+      </c>
+      <c r="N161" t="inlineStr">
+        <is>
+          <t>https://samenmeten.rivm.nl/vuurwerk/</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -9689,12 +9689,12 @@
       </c>
       <c r="M162" t="inlineStr">
         <is>
-          <t>https://www.samenmetenaanluchtkwaliteit.nl/oud-nieuw-2020-2021</t>
+          <t>https://www.samenmetenaanluchtkwaliteit.nl/</t>
         </is>
       </c>
       <c r="N162" t="inlineStr">
         <is>
-          <t>https://samenmeten.rivm.nl/vuurwerk/</t>
+          <t>https://samenmeten.rivm.nl/dataportaal/</t>
         </is>
       </c>
     </row>
@@ -9747,14 +9747,10 @@
       </c>
       <c r="M163" t="inlineStr">
         <is>
-          <t>https://www.samenmetenaanluchtkwaliteit.nl/</t>
-        </is>
-      </c>
-      <c r="N163" t="inlineStr">
-        <is>
-          <t>https://samenmeten.rivm.nl/dataportaal/</t>
-        </is>
-      </c>
+          <t>https://www.kwrwater.nl/projecten/citizen-science-praktijkpilot-versheid-water/</t>
+        </is>
+      </c>
+      <c r="N163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -9805,10 +9801,14 @@
       </c>
       <c r="M164" t="inlineStr">
         <is>
-          <t>https://www.kwrwater.nl/projecten/citizen-science-praktijkpilot-versheid-water/</t>
-        </is>
-      </c>
-      <c r="N164" t="inlineStr"/>
+          <t>https://www.samenmetenaanluchtkwaliteit.nl/vuurwerk-2016-2017</t>
+        </is>
+      </c>
+      <c r="N164" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://samenmeten.rivm.nl/dataportaal/  </t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -9859,12 +9859,12 @@
       </c>
       <c r="M165" t="inlineStr">
         <is>
-          <t>https://www.samenmetenaanluchtkwaliteit.nl/vuurwerk-2016-2017</t>
+          <t>https://www.samenmetenaanluchtkwaliteit.nl/luftdaten</t>
         </is>
       </c>
       <c r="N165" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://samenmeten.rivm.nl/dataportaal/  </t>
+          <t>https://samenmeten.rivm.nl/dataportaal/</t>
         </is>
       </c>
     </row>
@@ -9917,12 +9917,12 @@
       </c>
       <c r="M166" t="inlineStr">
         <is>
-          <t>https://www.samenmetenaanluchtkwaliteit.nl/luftdaten</t>
+          <t>https://www.samenmetenaanluchtkwaliteit.nl/burgermetingen-schiedam</t>
         </is>
       </c>
       <c r="N166" t="inlineStr">
         <is>
-          <t>https://samenmeten.rivm.nl/dataportaal/</t>
+          <t>https://www.webgispublisher.nl/schiedam/</t>
         </is>
       </c>
     </row>
@@ -10158,7 +10158,7 @@
       </c>
       <c r="N170" t="inlineStr">
         <is>
-          <t>https://www.schonerivieren.org/join/resultatenonderzoeken/</t>
+          <t>https://www.schonerivieren.org/join/resultaten-onderzoeken/</t>
         </is>
       </c>
     </row>
@@ -10220,7 +10220,7 @@
       </c>
       <c r="N171" t="inlineStr">
         <is>
-          <t>https://milieudefensie.nl/actueel/eindrapporthoegezondisonzelucht.pdf</t>
+          <t>https://milieudefensie.nl/actueel/eindrapport-hoe-gezond-is-onze-lucht.pdf</t>
         </is>
       </c>
     </row>
@@ -10282,7 +10282,7 @@
       </c>
       <c r="N172" t="inlineStr">
         <is>
-          <t>https://www.luchtmeetnetmaastricht.nl/maastricht/</t>
+          <t>https://www.luchtmeetnet-maastricht.nl/maastricht/</t>
         </is>
       </c>
     </row>
@@ -10576,7 +10576,7 @@
       </c>
       <c r="N177" t="inlineStr">
         <is>
-          <t>https://www.nioz.nl/en/about/cos/movementconnectivity/birdmovement/trackingmovementsofspoonbills/followspoonbillsfromthenetherlands</t>
+          <t>https://www.nioz.nl/en/about/cos/movement-connectivity/bird-movement/tracking-movements-of-spoonbills/follow-spoonbills-from-the-netherlands</t>
         </is>
       </c>
     </row>
@@ -10858,7 +10858,7 @@
       </c>
       <c r="N182" t="inlineStr">
         <is>
-          <t>https://www.clo.nl/indicatoren/nl1387libellen</t>
+          <t>https://www.clo.nl/indicatoren/nl1387-libellen</t>
         </is>
       </c>
     </row>
@@ -11426,7 +11426,7 @@
       </c>
       <c r="N192" t="inlineStr">
         <is>
-          <t>https://euring.org/dataandcodes/obtainingdata</t>
+          <t>https://euring.org/data-and-codes/obtaining-data</t>
         </is>
       </c>
     </row>
@@ -11836,7 +11836,7 @@
       </c>
       <c r="N199" t="inlineStr">
         <is>
-          <t>https://www.naturetoday.com/intl/nl/observations/mosquitoradar</t>
+          <t>https://www.naturetoday.com/intl/nl/observations/mosquito-radar</t>
         </is>
       </c>
     </row>
@@ -12245,7 +12245,7 @@
       </c>
       <c r="M206" t="inlineStr">
         <is>
-          <t>https://www.tuintelling.nl/evenementen/avondtelling</t>
+          <t>https://tuintelling.nl/evenementen/tuinvijvertelling</t>
         </is>
       </c>
       <c r="N206" t="inlineStr">
@@ -12303,12 +12303,12 @@
       </c>
       <c r="M207" t="inlineStr">
         <is>
-          <t>https://tuintelling.nl/evenementen/tuinvijvertelling</t>
+          <t>https://vogeltrekstation.nl/nl/onderzoek/monitoringsprojecten/pullen#quicktabs-pullen=0</t>
         </is>
       </c>
       <c r="N207" t="inlineStr">
         <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
+          <t>https://euring.org/data-and-codes/obtaining-data</t>
         </is>
       </c>
     </row>
@@ -12361,12 +12361,12 @@
       </c>
       <c r="M208" t="inlineStr">
         <is>
-          <t>https://vogeltrekstation.nl/nl/onderzoek/monitoringsprojecten/pullen#quicktabs-pullen=0</t>
+          <t>https://www.nationalebijentelling.nl/</t>
         </is>
       </c>
       <c r="N208" t="inlineStr">
         <is>
-          <t>https://euring.org/dataandcodes/obtainingdata</t>
+          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -12419,7 +12419,7 @@
       </c>
       <c r="M209" t="inlineStr">
         <is>
-          <t>https://www.nationalebijentelling.nl/</t>
+          <t>https://www.ravon.nl/Portals/2/Bestanden/Publicaties/Rapporten/2007.003k.pdf</t>
         </is>
       </c>
       <c r="N209" t="inlineStr">
@@ -12477,7 +12477,7 @@
       </c>
       <c r="M210" t="inlineStr">
         <is>
-          <t>https://www.ravon.nl/Portals/2/Bestanden/Publicaties/Rapporten/2007.003k.pdf</t>
+          <t>https://www.floron.nl/bermen</t>
         </is>
       </c>
       <c r="N210" t="inlineStr">
@@ -12535,7 +12535,7 @@
       </c>
       <c r="M211" t="inlineStr">
         <is>
-          <t>https://www.floron.nl/bermen</t>
+          <t>https://www.sovon.nl/nl/actueel/nieuws/lijsters-en-bessen-tellen</t>
         </is>
       </c>
       <c r="N211" t="inlineStr">
@@ -12593,7 +12593,7 @@
       </c>
       <c r="M212" t="inlineStr">
         <is>
-          <t>https://www.sovon.nl/nl/actueel/nieuws/lijsters-en-bessen-tellen</t>
+          <t>https://www.vleermuis.net/</t>
         </is>
       </c>
       <c r="N212" t="inlineStr">
@@ -12651,7 +12651,7 @@
       </c>
       <c r="M213" t="inlineStr">
         <is>
-          <t>https://www.vleermuis.net/</t>
+          <t>https://www.sovon.nl/nl/MUS</t>
         </is>
       </c>
       <c r="N213" t="inlineStr">
@@ -12709,14 +12709,10 @@
       </c>
       <c r="M214" t="inlineStr">
         <is>
-          <t>https://www.sovon.nl/nl/MUS</t>
-        </is>
-      </c>
-      <c r="N214" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
-        </is>
-      </c>
+          <t>https://submit.cr-birding.org/page/who_are_we/</t>
+        </is>
+      </c>
+      <c r="N214" t="inlineStr"/>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -12767,10 +12763,14 @@
       </c>
       <c r="M215" t="inlineStr">
         <is>
-          <t>https://submit.cr-birding.org/page/who_are_we/</t>
-        </is>
-      </c>
-      <c r="N215" t="inlineStr"/>
+          <t>https://www.tuintelling.nl/evenementen/avondtelling</t>
+        </is>
+      </c>
+      <c r="N215" t="inlineStr">
+        <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -12826,7 +12826,7 @@
       </c>
       <c r="N216" t="inlineStr">
         <is>
-          <t>https://euring.org/dataandcodes/obtainingdata</t>
+          <t>https://euring.org/data-and-codes/obtaining-data</t>
         </is>
       </c>
     </row>
@@ -13270,7 +13270,7 @@
       </c>
       <c r="N224" t="inlineStr">
         <is>
-          <t>https://euring.org/dataandcodes/obtainingdata</t>
+          <t>https://euring.org/data-and-codes/obtaining-data</t>
         </is>
       </c>
     </row>
@@ -13614,7 +13614,7 @@
       </c>
       <c r="N230" t="inlineStr">
         <is>
-          <t>https://www.cbs.nl/nlnl/nieuws/2017/01/verspreidinginvasieveplantensoortentoegenomen en https://www.clo.nl/indicatoren/nl1398invasieveplantensoorten</t>
+          <t>https://www.cbs.nl/nl-nl/nieuws/2017/01/verspreiding-invasieve-plantensoorten-toegenomen en https://www.clo.nl/indicatoren/nl1398-invasieve-plantensoorten</t>
         </is>
       </c>
     </row>
@@ -13672,7 +13672,7 @@
       </c>
       <c r="N231" t="inlineStr">
         <is>
-          <t>https://euring.org/dataandcodes/obtainingdata</t>
+          <t>https://euring.org/data-and-codes/obtaining-data</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Change csv separator to "|"
</commit_message>
<xml_diff>
--- a/data/citizen-science-projects-nl.xlsx
+++ b/data/citizen-science-projects-nl.xlsx
@@ -507,12 +507,12 @@
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
+          <t>data_url</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
           <t>project_information_url</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>data_url</t>
         </is>
       </c>
     </row>
@@ -573,12 +573,12 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
           <t>https://www.archeologieleeft.nl/archeosuccessen/erfgoed-gezocht/</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -637,12 +637,12 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
           <t>https://www.universiteitleiden.nl/citizensciencelab/projecten/erfgoed-gezocht</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -697,12 +697,12 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
           <t>https://www.universiteitleiden.nl/nieuws/2020/04/erfgoed-gezocht-junior-kinderen-speuren-vanuit-huis-mee-met-archeologen</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -757,12 +757,12 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
+          <t>https://www.griepencorona.nl/resultaten/</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
           <t>https://www.griepencorona.nl/het-project/</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>https://www.griepencorona.nl/resultaten/</t>
         </is>
       </c>
     </row>
@@ -821,12 +821,12 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
           <t>https://www.jagersvereniging.nl/downloads/bestuurdersdocumenten/telprotocol-zomerganzentelling/</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -881,12 +881,12 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
           <t>https://www.rivm.nl/rivm/kennis-en-kunde/strategisch-programma-rivm/spr-2015-2018/integrale-risicobeoordeling/ik-heb-nu-last-app</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -941,12 +941,12 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
           <t>https://www.mycardio.nl/</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -1063,12 +1063,12 @@
       </c>
       <c r="O10" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
           <t>https://www.nemokennislink.nl/publicaties/doe-mee-aan-de-grote-griepmeting/</t>
-        </is>
-      </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -1183,12 +1183,12 @@
       </c>
       <c r="O12" t="inlineStr">
         <is>
+          <t>https://www.globe.gov/globe-data/visualize-and-retrieve-data</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
           <t>https://globenederland.nl/onderzoeksproject/aerosolen/#info</t>
-        </is>
-      </c>
-      <c r="P12" t="inlineStr">
-        <is>
-          <t>https://www.globe.gov/globe-data/visualize-and-retrieve-data</t>
         </is>
       </c>
     </row>
@@ -1247,12 +1247,12 @@
       </c>
       <c r="O13" t="inlineStr">
         <is>
+          <t>https://www.globe.gov/globe-data/visualize-and-retrieve-data</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
           <t>https://globenederland.nl/onderzoeksproject/smap/#info</t>
-        </is>
-      </c>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>https://www.globe.gov/globe-data/visualize-and-retrieve-data</t>
         </is>
       </c>
     </row>
@@ -1307,12 +1307,12 @@
       </c>
       <c r="O14" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
           <t>https://www.iedereenwetenschapper.be/projects/download-je-eigen-deeltjesdetector</t>
-        </is>
-      </c>
-      <c r="P14" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -1367,12 +1367,12 @@
       </c>
       <c r="O15" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
           <t>https://www.iedereenwetenschapper.be/projects/bekijk-de-aarde-vanuit-de-ruimte</t>
-        </is>
-      </c>
-      <c r="P15" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -1435,12 +1435,12 @@
       </c>
       <c r="O16" t="inlineStr">
         <is>
+          <t>http://www.wesense.info/en/maps.html</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
           <t>http://www.wesense.info/en/index.html</t>
-        </is>
-      </c>
-      <c r="P16" t="inlineStr">
-        <is>
-          <t>http://www.wesense.info/en/maps.html</t>
         </is>
       </c>
     </row>
@@ -1497,12 +1497,12 @@
       </c>
       <c r="O17" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
           <t>https://ronaldbierings.com/over-zicht-op-licht/</t>
-        </is>
-      </c>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -1561,12 +1561,12 @@
       </c>
       <c r="O18" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
           <t>https://www.rug.nl/sciencelinx/maatschappij/curious</t>
-        </is>
-      </c>
-      <c r="P18" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -1627,12 +1627,12 @@
       </c>
       <c r="O19" t="inlineStr">
         <is>
+          <t>http://personagebank.nl/resultaten/</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
           <t>http://personagebank.nl/</t>
-        </is>
-      </c>
-      <c r="P19" t="inlineStr">
-        <is>
-          <t>http://personagebank.nl/resultaten/</t>
         </is>
       </c>
     </row>
@@ -1687,12 +1687,12 @@
       </c>
       <c r="O20" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
           <t>https://www.rivm.nl/burgerwetenschap/shift-diets</t>
-        </is>
-      </c>
-      <c r="P20" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -1749,12 +1749,12 @@
       </c>
       <c r="O21" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
           <t>https://www.iedereenwetenschapper.be/projects/hoe-snel-herken-jij-een-liedje</t>
-        </is>
-      </c>
-      <c r="P21" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -1815,12 +1815,12 @@
       </c>
       <c r="O22" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
           <t>http://www.kijkeengezondewijk.nl/#/info</t>
-        </is>
-      </c>
-      <c r="P22" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -1935,12 +1935,12 @@
       </c>
       <c r="O24" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
           <t>https://www.wetenschapsknooppunten.nl/alle-scholen-verzamelen/citizen-science/</t>
-        </is>
-      </c>
-      <c r="P24" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -1997,12 +1997,12 @@
       </c>
       <c r="O25" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
           <t>https://www.nemokennislink.nl/publicaties/zie-ik-spoken/</t>
-        </is>
-      </c>
-      <c r="P25" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -2057,12 +2057,12 @@
       </c>
       <c r="O26" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
           <t>https://woordwaark.nl/stemmen/</t>
-        </is>
-      </c>
-      <c r="P26" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -2121,12 +2121,12 @@
       </c>
       <c r="O27" t="inlineStr">
         <is>
+          <t>http://stimmen.nl/uitspraakkaarten/</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
           <t>http://stimmen.nl/</t>
-        </is>
-      </c>
-      <c r="P27" t="inlineStr">
-        <is>
-          <t>http://stimmen.nl/uitspraakkaarten/</t>
         </is>
       </c>
     </row>
@@ -2181,12 +2181,12 @@
       </c>
       <c r="O28" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
           <t>https://www.tudelft.nl/scd/waterlab/doe-mee-aan-onderzoek/project-6-nationale-plasticwatch</t>
-        </is>
-      </c>
-      <c r="P28" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -2241,12 +2241,12 @@
       </c>
       <c r="O29" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
           <t xml:space="preserve">https://www.floron.nl/meedoen/het-nieuwe-strepen </t>
-        </is>
-      </c>
-      <c r="P29" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -2301,12 +2301,12 @@
       </c>
       <c r="O30" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/bhic_repnot</t>
-        </is>
-      </c>
-      <c r="P30" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -2363,12 +2363,12 @@
       </c>
       <c r="O31" t="inlineStr">
         <is>
+          <t>https://www.wiewaswie.nl/</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/2/project/kha</t>
-        </is>
-      </c>
-      <c r="P31" t="inlineStr">
-        <is>
-          <t>https://www.wiewaswie.nl/</t>
         </is>
       </c>
     </row>
@@ -2423,12 +2423,12 @@
       </c>
       <c r="O32" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/sahm_index_bevolkingsregisters</t>
-        </is>
-      </c>
-      <c r="P32" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -2483,12 +2483,12 @@
       </c>
       <c r="O33" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/wiewaswie_bvr</t>
-        </is>
-      </c>
-      <c r="P33" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -2545,12 +2545,12 @@
       </c>
       <c r="O34" t="inlineStr">
         <is>
+          <t>https://www.zeeuwsarchief.nl/zeeuwen-gezocht/</t>
+        </is>
+      </c>
+      <c r="P34" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/picvh_zar</t>
-        </is>
-      </c>
-      <c r="P34" t="inlineStr">
-        <is>
-          <t>https://www.zeeuwsarchief.nl/zeeuwen-gezocht/</t>
         </is>
       </c>
     </row>
@@ -2605,12 +2605,12 @@
       </c>
       <c r="O35" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P35" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/mai_tagging</t>
-        </is>
-      </c>
-      <c r="P35" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -2667,12 +2667,12 @@
       </c>
       <c r="O36" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P36" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/status/closed/project/gda_2</t>
-        </is>
-      </c>
-      <c r="P36" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -2729,12 +2729,12 @@
       </c>
       <c r="O37" t="inlineStr">
         <is>
+          <t>http://www.bhic.nl/onderzoeken/hulp-bij-onderzoek/gevangenisarchieven</t>
+        </is>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/3/project/bhic_strafgevangenissen</t>
-        </is>
-      </c>
-      <c r="P37" t="inlineStr">
-        <is>
-          <t>http://www.bhic.nl/onderzoeken/hulp-bij-onderzoek/gevangenisarchieven</t>
         </is>
       </c>
     </row>
@@ -2791,12 +2791,12 @@
       </c>
       <c r="O38" t="inlineStr">
         <is>
+          <t>https://archief.amsterdam/inventarissen/details/10035</t>
+        </is>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/amsterdam_kaarten</t>
-        </is>
-      </c>
-      <c r="P38" t="inlineStr">
-        <is>
-          <t>https://archief.amsterdam/inventarissen/details/10035</t>
         </is>
       </c>
     </row>
@@ -2853,12 +2853,12 @@
       </c>
       <c r="O39" t="inlineStr">
         <is>
+          <t>https://www.regionaalarchiefalkmaar.nl/collecties/beelden/beelden-2/?q=kaarten&amp;mode=gallery&amp;view=horizontal</t>
+        </is>
+      </c>
+      <c r="P39" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/raa</t>
-        </is>
-      </c>
-      <c r="P39" t="inlineStr">
-        <is>
-          <t>https://www.regionaalarchiefalkmaar.nl/collecties/beelden/beelden-2/?q=kaarten&amp;mode=gallery&amp;view=horizontal</t>
         </is>
       </c>
     </row>
@@ -2913,12 +2913,12 @@
       </c>
       <c r="O40" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P40" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/gra_tagging_vanderveen</t>
-        </is>
-      </c>
-      <c r="P40" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -2975,12 +2975,12 @@
       </c>
       <c r="O41" t="inlineStr">
         <is>
+          <t>https://studiezaal.nijmegen.nl/zoeken.php</t>
+        </is>
+      </c>
+      <c r="P41" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/2/project/picvh_han_nijmegen</t>
-        </is>
-      </c>
-      <c r="P41" t="inlineStr">
-        <is>
-          <t>https://studiezaal.nijmegen.nl/zoeken.php</t>
         </is>
       </c>
     </row>
@@ -3037,12 +3037,12 @@
       </c>
       <c r="O42" t="inlineStr">
         <is>
+          <t>https://www.westfriesarchief.nl/onderzoek/zoeken/personen</t>
+        </is>
+      </c>
+      <c r="P42" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/wfg_index</t>
-        </is>
-      </c>
-      <c r="P42" t="inlineStr">
-        <is>
-          <t>https://www.westfriesarchief.nl/onderzoek/zoeken/personen</t>
         </is>
       </c>
     </row>
@@ -3097,12 +3097,12 @@
       </c>
       <c r="O43" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P43" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/run_slavenregisters</t>
-        </is>
-      </c>
-      <c r="P43" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -3159,12 +3159,12 @@
       </c>
       <c r="O44" t="inlineStr">
         <is>
+          <t>https://www.muziekschatten.nl/omroepmuziek#eyJ0eXBlIjoibGlzdCIsImF2YWlsYWJpbGl0eSI6W10sImNvbXBvc2VyIjpbXSwiY2F0ZWdvcnkiOltdLCJnZW5yZSI6W10sImNvbGxlY3Rpb24iOltdLCJpbnN0cnVtZW50IjpbXSwiZmFjZXRzIjp7ImF2YWlsYWJpbGl0eSI6eyJ0ZXJtcyI6eyJmaWVsZCI6ImF2YWlsYWJpbGl0eSIsInNpemUiOjEwMH19LCJjb21wb3NlciI6eyJ0ZXJtcyI6eyJmaWVsZCI6ImNvbXBvc2VyIiwic2l6ZSI6MTAwfX0sImNhdGVnb3J5Ijp7InRlcm1zIjp7ImZpZWxkIjoiY2F0ZWdvcnkiLCJzaXplIjoxMDB9fSwiZ2VucmUiOnsidGVybXMiOnsiZmllbGQiOiJnZW5yZSIsInNpemUiOjEwMH19LCJjb2xsZWN0aW9uIjp7InRlcm1zIjp7ImZpZWxkIjoiY29sbGVjdGlvbiIsInNpemUiOjEwMH19LCJ1bmRlZmluZWQiOnsidGVybXMiOnt9fX19</t>
+        </is>
+      </c>
+      <c r="P44" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/som_index</t>
-        </is>
-      </c>
-      <c r="P44" t="inlineStr">
-        <is>
-          <t>https://www.muziekschatten.nl/omroepmuziek#eyJ0eXBlIjoibGlzdCIsImF2YWlsYWJpbGl0eSI6W10sImNvbXBvc2VyIjpbXSwiY2F0ZWdvcnkiOltdLCJnZW5yZSI6W10sImNvbGxlY3Rpb24iOltdLCJpbnN0cnVtZW50IjpbXSwiZmFjZXRzIjp7ImF2YWlsYWJpbGl0eSI6eyJ0ZXJtcyI6eyJmaWVsZCI6ImF2YWlsYWJpbGl0eSIsInNpemUiOjEwMH19LCJjb21wb3NlciI6eyJ0ZXJtcyI6eyJmaWVsZCI6ImNvbXBvc2VyIiwic2l6ZSI6MTAwfX0sImNhdGVnb3J5Ijp7InRlcm1zIjp7ImZpZWxkIjoiY2F0ZWdvcnkiLCJzaXplIjoxMDB9fSwiZ2VucmUiOnsidGVybXMiOnsiZmllbGQiOiJnZW5yZSIsInNpemUiOjEwMH19LCJjb2xsZWN0aW9uIjp7InRlcm1zIjp7ImZpZWxkIjoiY29sbGVjdGlvbiIsInNpemUiOjEwMH19LCJ1bmRlZmluZWQiOnsidGVybXMiOnt9fX19</t>
         </is>
       </c>
     </row>
@@ -3221,12 +3221,12 @@
       </c>
       <c r="O45" t="inlineStr">
         <is>
+          <t>https://www.zeeuwsarchief.nl/onderzoek-het-zelf/</t>
+        </is>
+      </c>
+      <c r="P45" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/picvh_zar_index_terneuzenaxel</t>
-        </is>
-      </c>
-      <c r="P45" t="inlineStr">
-        <is>
-          <t>https://www.zeeuwsarchief.nl/onderzoek-het-zelf/</t>
         </is>
       </c>
     </row>
@@ -3283,12 +3283,12 @@
       </c>
       <c r="O46" t="inlineStr">
         <is>
+          <t>https://search.iisg.amsterdam/Record/ARCH00210</t>
+        </is>
+      </c>
+      <c r="P46" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/mbi</t>
-        </is>
-      </c>
-      <c r="P46" t="inlineStr">
-        <is>
-          <t>https://search.iisg.amsterdam/Record/ARCH00210</t>
         </is>
       </c>
     </row>
@@ -3345,12 +3345,12 @@
       </c>
       <c r="O47" t="inlineStr">
         <is>
+          <t>https://archief.amsterdam/uitleg/indexen/41-pensioenkaarten-1894-1915?utm_source=OpenArchieven&amp;utm_medium=browser&amp;utm_campaign=OpenData</t>
+        </is>
+      </c>
+      <c r="P47" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/2/project/amsterdam_pensioen</t>
-        </is>
-      </c>
-      <c r="P47" t="inlineStr">
-        <is>
-          <t>https://archief.amsterdam/uitleg/indexen/41-pensioenkaarten-1894-1915?utm_source=OpenArchieven&amp;utm_medium=browser&amp;utm_campaign=OpenData</t>
         </is>
       </c>
     </row>
@@ -3405,12 +3405,12 @@
       </c>
       <c r="O48" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P48" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/legermuseum</t>
-        </is>
-      </c>
-      <c r="P48" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -3467,12 +3467,12 @@
       </c>
       <c r="O49" t="inlineStr">
         <is>
+          <t>https://archief.amsterdam/indexen/persons</t>
+        </is>
+      </c>
+      <c r="P49" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/2/project/amsterdam_13442</t>
-        </is>
-      </c>
-      <c r="P49" t="inlineStr">
-        <is>
-          <t>https://archief.amsterdam/indexen/persons</t>
         </is>
       </c>
     </row>
@@ -3527,12 +3527,12 @@
       </c>
       <c r="O50" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P50" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/wfg_transcription_notarieel</t>
-        </is>
-      </c>
-      <c r="P50" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -3589,12 +3589,12 @@
       </c>
       <c r="O51" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P51" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/picvh_run</t>
-        </is>
-      </c>
-      <c r="P51" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -3651,12 +3651,12 @@
       </c>
       <c r="O52" t="inlineStr">
         <is>
+          <t>https://www.samh.nl/</t>
+        </is>
+      </c>
+      <c r="P52" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/sahm_indexing_persons</t>
-        </is>
-      </c>
-      <c r="P52" t="inlineStr">
-        <is>
-          <t>https://www.samh.nl/</t>
         </is>
       </c>
     </row>
@@ -3711,12 +3711,12 @@
       </c>
       <c r="O53" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P53" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/vua_train_kronieken_transkribus</t>
-        </is>
-      </c>
-      <c r="P53" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -3773,12 +3773,12 @@
       </c>
       <c r="O54" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P54" t="inlineStr">
+        <is>
           <t>https://www.iedereenwetenschapper.be/projects/duik-historisch-amsterdam</t>
-        </is>
-      </c>
-      <c r="P54" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -3833,12 +3833,12 @@
       </c>
       <c r="O55" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P55" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/rar_index_repertoria</t>
-        </is>
-      </c>
-      <c r="P55" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -3895,12 +3895,12 @@
       </c>
       <c r="O56" t="inlineStr">
         <is>
+          <t>https://www.archiefeemland.nl/</t>
+        </is>
+      </c>
+      <c r="P56" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/gam_gezinskaarten</t>
-        </is>
-      </c>
-      <c r="P56" t="inlineStr">
-        <is>
-          <t>https://www.archiefeemland.nl/</t>
         </is>
       </c>
     </row>
@@ -3957,12 +3957,12 @@
       </c>
       <c r="O57" t="inlineStr">
         <is>
+          <t>https://archief.amsterdam/indexen/persons?f=%7B%22search_i_datum%22:%7B%22v%22:%5B%2218640000%22,%2218749999%22%5D,%22d%22:%221864%20-%201874%22%7D%7D</t>
+        </is>
+      </c>
+      <c r="P57" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/amsterdam_index_bvr3</t>
-        </is>
-      </c>
-      <c r="P57" t="inlineStr">
-        <is>
-          <t>https://archief.amsterdam/indexen/persons?f=%7B%22search_i_datum%22:%7B%22v%22:%5B%2218640000%22,%2218749999%22%5D,%22d%22:%221864%20-%201874%22%7D%7D</t>
         </is>
       </c>
     </row>
@@ -4017,12 +4017,12 @@
       </c>
       <c r="O58" t="inlineStr">
         <is>
+          <t>https://noord-hollandsarchief.nl/beelden/beeldbank/?fq%5B%5D=search_s_afbeelding:%22Ja%22&amp;mode=gallery&amp;view=horizontal&amp;sort=random%7B1612191303970%7D%20asc</t>
+        </is>
+      </c>
+      <c r="P58" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/ranh_tagselection_deboer</t>
-        </is>
-      </c>
-      <c r="P58" t="inlineStr">
-        <is>
-          <t>https://noord-hollandsarchief.nl/beelden/beeldbank/?fq%5B%5D=search_s_afbeelding:%22Ja%22&amp;mode=gallery&amp;view=horizontal&amp;sort=random%7B1612191303970%7D%20asc</t>
         </is>
       </c>
     </row>
@@ -4079,12 +4079,12 @@
       </c>
       <c r="O59" t="inlineStr">
         <is>
+          <t>https://www.kabk.nl/alumni/bachelor-beeldende-kunst</t>
+        </is>
+      </c>
+      <c r="P59" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/3/project/kabk</t>
-        </is>
-      </c>
-      <c r="P59" t="inlineStr">
-        <is>
-          <t>https://www.kabk.nl/alumni/bachelor-beeldende-kunst</t>
         </is>
       </c>
     </row>
@@ -4139,12 +4139,12 @@
       </c>
       <c r="O60" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P60" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/mei</t>
-        </is>
-      </c>
-      <c r="P60" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -4201,12 +4201,12 @@
       </c>
       <c r="O61" t="inlineStr">
         <is>
+          <t>https://archief.amsterdam/indexen/persons?f=%7B%22search_i_datum%22:%7B%22v%22:%5B%2218740000%22,%2218939999%22%5D,%22d%22:%221874%20-%201893%22%7D%7D</t>
+        </is>
+      </c>
+      <c r="P61" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/2/project/amsterdam_bvr</t>
-        </is>
-      </c>
-      <c r="P61" t="inlineStr">
-        <is>
-          <t>https://archief.amsterdam/indexen/persons?f=%7B%22search_i_datum%22:%7B%22v%22:%5B%2218740000%22,%2218939999%22%5D,%22d%22:%221874%20-%201893%22%7D%7D</t>
         </is>
       </c>
     </row>
@@ -4263,12 +4263,12 @@
       </c>
       <c r="O62" t="inlineStr">
         <is>
+          <t>https://www.beeldbankgroningen.nl/beelden/?mode=gallery&amp;view=horizontal&amp;sort=random%7B1541835054895%7D%20asc&amp;page=1&amp;fq%5B%5D=search_t_gegeorefereerd:%22ja%22&amp;reverse=0&amp;filterAction</t>
+        </is>
+      </c>
+      <c r="P62" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/gra_kaarten</t>
-        </is>
-      </c>
-      <c r="P62" t="inlineStr">
-        <is>
-          <t>https://www.beeldbankgroningen.nl/beelden/?mode=gallery&amp;view=horizontal&amp;sort=random%7B1541835054895%7D%20asc&amp;page=1&amp;fq%5B%5D=search_t_gegeorefereerd:%22ja%22&amp;reverse=0&amp;filterAction</t>
         </is>
       </c>
     </row>
@@ -4323,12 +4323,12 @@
       </c>
       <c r="O63" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P63" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/tlb_index</t>
-        </is>
-      </c>
-      <c r="P63" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -4385,12 +4385,12 @@
       </c>
       <c r="O64" t="inlineStr">
         <is>
+          <t>https://archief.amsterdam/uitleg/indexen/42-patientenregisters-1818-1899?utm_source=OpenArchieven&amp;utm_medium=browser&amp;utm_campaign=OpenData</t>
+        </is>
+      </c>
+      <c r="P64" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/2/project/amsterdam_patient</t>
-        </is>
-      </c>
-      <c r="P64" t="inlineStr">
-        <is>
-          <t>https://archief.amsterdam/uitleg/indexen/42-patientenregisters-1818-1899?utm_source=OpenArchieven&amp;utm_medium=browser&amp;utm_campaign=OpenData</t>
         </is>
       </c>
     </row>
@@ -4447,12 +4447,12 @@
       </c>
       <c r="O65" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P65" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/ja_ik_wil</t>
-        </is>
-      </c>
-      <c r="P65" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -4509,12 +4509,12 @@
       </c>
       <c r="O66" t="inlineStr">
         <is>
+          <t>https://www.geldersarchief.nl/bronnen/archieven/?mivast=37&amp;miadt=37&amp;mizig=128&amp;miview=tbl&amp;milang=nl&amp;micols=1&amp;misort=last_mod%7Cdesc&amp;mib1=113</t>
+        </is>
+      </c>
+      <c r="P66" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/2/project/gda</t>
-        </is>
-      </c>
-      <c r="P66" t="inlineStr">
-        <is>
-          <t>https://www.geldersarchief.nl/bronnen/archieven/?mivast=37&amp;miadt=37&amp;mizig=128&amp;miview=tbl&amp;milang=nl&amp;micols=1&amp;misort=last_mod%7Cdesc&amp;mib1=113</t>
         </is>
       </c>
     </row>
@@ -4569,12 +4569,12 @@
       </c>
       <c r="O67" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P67" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/cbg_index_hal</t>
-        </is>
-      </c>
-      <c r="P67" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -4629,12 +4629,12 @@
       </c>
       <c r="O68" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P68" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/nfm_tagging_photos</t>
-        </is>
-      </c>
-      <c r="P68" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -4689,12 +4689,12 @@
       </c>
       <c r="O69" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P69" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/leiden_na1</t>
-        </is>
-      </c>
-      <c r="P69" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -4751,12 +4751,12 @@
       </c>
       <c r="O70" t="inlineStr">
         <is>
+          <t>https://www.openarch.nl/indexen/9/militieregisters?lang=nl</t>
+        </is>
+      </c>
+      <c r="P70" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/3/project/militieregisters</t>
-        </is>
-      </c>
-      <c r="P70" t="inlineStr">
-        <is>
-          <t>https://www.openarch.nl/indexen/9/militieregisters?lang=nl</t>
         </is>
       </c>
     </row>
@@ -4813,12 +4813,12 @@
       </c>
       <c r="O71" t="inlineStr">
         <is>
+          <t>https://archief.amsterdam/beeldbank/?mode=gallery&amp;view=horizontal&amp;q=het%20vrije%20volk&amp;page=1&amp;reverse=0</t>
+        </is>
+      </c>
+      <c r="P71" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/amsterdam_vrije_volk</t>
-        </is>
-      </c>
-      <c r="P71" t="inlineStr">
-        <is>
-          <t>https://archief.amsterdam/beeldbank/?mode=gallery&amp;view=horizontal&amp;q=het%20vrije%20volk&amp;page=1&amp;reverse=0</t>
         </is>
       </c>
     </row>
@@ -4873,12 +4873,12 @@
       </c>
       <c r="O72" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P72" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/gda_index_huwelijk</t>
-        </is>
-      </c>
-      <c r="P72" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -4933,12 +4933,12 @@
       </c>
       <c r="O73" t="inlineStr">
         <is>
+          <t>https://www.wiewaswie.nl/</t>
+        </is>
+      </c>
+      <c r="P73" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/brd_index_repertoria</t>
-        </is>
-      </c>
-      <c r="P73" t="inlineStr">
-        <is>
-          <t>https://www.wiewaswie.nl/</t>
         </is>
       </c>
     </row>
@@ -4993,12 +4993,12 @@
       </c>
       <c r="O74" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P74" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/frl</t>
-        </is>
-      </c>
-      <c r="P74" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -5055,12 +5055,12 @@
       </c>
       <c r="O75" t="inlineStr">
         <is>
+          <t>https://www.naturalis.nl/collectie</t>
+        </is>
+      </c>
+      <c r="P75" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/3/project/nat_nbc</t>
-        </is>
-      </c>
-      <c r="P75" t="inlineStr">
-        <is>
-          <t>https://www.naturalis.nl/collectie</t>
         </is>
       </c>
     </row>
@@ -5117,12 +5117,12 @@
       </c>
       <c r="O76" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P76" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/status/closed/project/bhic_strafgevangenissen_2</t>
-        </is>
-      </c>
-      <c r="P76" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -5177,12 +5177,12 @@
       </c>
       <c r="O77" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P77" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/huy_correct_resoluties_transkribus</t>
-        </is>
-      </c>
-      <c r="P77" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -5239,12 +5239,12 @@
       </c>
       <c r="O78" t="inlineStr">
         <is>
+          <t>https://studiezaal.nijmegen.nl/zoeken.php?zoeken[beschrijvingsgroepen][2145654597]=2145654597</t>
+        </is>
+      </c>
+      <c r="P78" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/3/project/nijmegen_bvr</t>
-        </is>
-      </c>
-      <c r="P78" t="inlineStr">
-        <is>
-          <t>https://studiezaal.nijmegen.nl/zoeken.php?zoeken[beschrijvingsgroepen][2145654597]=2145654597</t>
         </is>
       </c>
     </row>
@@ -5299,12 +5299,12 @@
       </c>
       <c r="O79" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P79" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/picvh_bhic_bevolkingsregister</t>
-        </is>
-      </c>
-      <c r="P79" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -5359,12 +5359,12 @@
       </c>
       <c r="O80" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P80" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/amsterdam_correct_notarieel_transkribus</t>
-        </is>
-      </c>
-      <c r="P80" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -5419,12 +5419,12 @@
       </c>
       <c r="O81" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P81" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/hga_index_gezinskaarten</t>
-        </is>
-      </c>
-      <c r="P81" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -5479,12 +5479,12 @@
       </c>
       <c r="O82" t="inlineStr">
         <is>
+          <t>https://archief.amsterdam/indexen/persons</t>
+        </is>
+      </c>
+      <c r="P82" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/amsterdam_index_vreemdelingenkaarten</t>
-        </is>
-      </c>
-      <c r="P82" t="inlineStr">
-        <is>
-          <t>https://archief.amsterdam/indexen/persons</t>
         </is>
       </c>
     </row>
@@ -5541,12 +5541,12 @@
       </c>
       <c r="O83" t="inlineStr">
         <is>
+          <t>https://www.archieven.nl/mi/1648/?mivast=1648&amp;mizig=0&amp;miadt=1648&amp;miview=lst&amp;mizk_alle=trefwoord:Bevolkingsregistratiehttps://www.archieven.nl/mi/1648/?mivast=1648&amp;mizig=0&amp;miadt=1648&amp;miview=lst&amp;mizk_alle=trefwoord:Bevolkingsregistratie</t>
+        </is>
+      </c>
+      <c r="P83" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/2/project/swl_bvr</t>
-        </is>
-      </c>
-      <c r="P83" t="inlineStr">
-        <is>
-          <t>https://www.archieven.nl/mi/1648/?mivast=1648&amp;mizig=0&amp;miadt=1648&amp;miview=lst&amp;mizk_alle=trefwoord:Bevolkingsregistratiehttps://www.archieven.nl/mi/1648/?mivast=1648&amp;mizig=0&amp;miadt=1648&amp;miview=lst&amp;mizk_alle=trefwoord:Bevolkingsregistratie</t>
         </is>
       </c>
     </row>
@@ -5601,12 +5601,12 @@
       </c>
       <c r="O84" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P84" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/ranh_index</t>
-        </is>
-      </c>
-      <c r="P84" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -5661,12 +5661,12 @@
       </c>
       <c r="O85" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P85" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/hfl_tagging_rijpcollectie</t>
-        </is>
-      </c>
-      <c r="P85" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -5723,12 +5723,12 @@
       </c>
       <c r="O86" t="inlineStr">
         <is>
+          <t>https://archief.amsterdam/uitleg/indexen/65-bevolkingsregister-overgenomen-delen-1892-1920?utm_source=OpenArchieven&amp;utm_medium=browser&amp;utm_campaign=OpenData</t>
+        </is>
+      </c>
+      <c r="P86" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/3/project/amsterdam_ogd</t>
-        </is>
-      </c>
-      <c r="P86" t="inlineStr">
-        <is>
-          <t>https://archief.amsterdam/uitleg/indexen/65-bevolkingsregister-overgenomen-delen-1892-1920?utm_source=OpenArchieven&amp;utm_medium=browser&amp;utm_campaign=OpenData</t>
         </is>
       </c>
     </row>
@@ -5783,12 +5783,12 @@
       </c>
       <c r="O87" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P87" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/vua_annoteer_kronieken_transkribus</t>
-        </is>
-      </c>
-      <c r="P87" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -5845,12 +5845,12 @@
       </c>
       <c r="O88" t="inlineStr">
         <is>
+          <t>https://www.huisvandenijmeegsegeschiedenis.nl/info/Deelnemersregistratie_Vierdaagse</t>
+        </is>
+      </c>
+      <c r="P88" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/2/project/picvh_han</t>
-        </is>
-      </c>
-      <c r="P88" t="inlineStr">
-        <is>
-          <t>https://www.huisvandenijmeegsegeschiedenis.nl/info/Deelnemersregistratie_Vierdaagse</t>
         </is>
       </c>
     </row>
@@ -5907,12 +5907,12 @@
       </c>
       <c r="O89" t="inlineStr">
         <is>
+          <t>https://www.drentsarchief.nl/onderzoeken/zoektips/stamboomonderzoek</t>
+        </is>
+      </c>
+      <c r="P89" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/dre_index_inschrijvingsregisters</t>
-        </is>
-      </c>
-      <c r="P89" t="inlineStr">
-        <is>
-          <t>https://www.drentsarchief.nl/onderzoeken/zoektips/stamboomonderzoek</t>
         </is>
       </c>
     </row>
@@ -5967,12 +5967,12 @@
       </c>
       <c r="O90" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P90" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/utrecht_transcription_notarieel</t>
-        </is>
-      </c>
-      <c r="P90" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -6029,12 +6029,12 @@
       </c>
       <c r="O91" t="inlineStr">
         <is>
+          <t>https://www.archieven.nl/nl/zoeken?mivast=0&amp;mizig=0&amp;miadt=0&amp;milang=nl&amp;misort=score%7Cdesc&amp;mizk_alle=deventer&amp;mif3=2&amp;miview=lst</t>
+        </is>
+      </c>
+      <c r="P91" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/3/project/sad</t>
-        </is>
-      </c>
-      <c r="P91" t="inlineStr">
-        <is>
-          <t>https://www.archieven.nl/nl/zoeken?mivast=0&amp;mizig=0&amp;miadt=0&amp;milang=nl&amp;misort=score%7Cdesc&amp;mizk_alle=deventer&amp;mif3=2&amp;miview=lst</t>
         </is>
       </c>
     </row>
@@ -6089,12 +6089,12 @@
       </c>
       <c r="O92" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P92" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/utr_index_bvr_1850_1889</t>
-        </is>
-      </c>
-      <c r="P92" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -6149,12 +6149,12 @@
       </c>
       <c r="O93" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P93" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/zaa_index_gaarder</t>
-        </is>
-      </c>
-      <c r="P93" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -6207,12 +6207,12 @@
       </c>
       <c r="O94" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P94" t="inlineStr">
+        <is>
           <t>https://www.iedereenwetenschapper.be/projects/reis-terug-de-tijd</t>
-        </is>
-      </c>
-      <c r="P94" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -6267,12 +6267,12 @@
       </c>
       <c r="O95" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P95" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/afc_tagging_2</t>
-        </is>
-      </c>
-      <c r="P95" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -6329,12 +6329,12 @@
       </c>
       <c r="O96" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P96" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/zaa_index_bron</t>
-        </is>
-      </c>
-      <c r="P96" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -6391,12 +6391,12 @@
       </c>
       <c r="O97" t="inlineStr">
         <is>
+          <t>https://archief.amsterdam/uitleg/indexen/67-bevolkingsregister-geannexeerde-gemeenten-1830-1921</t>
+        </is>
+      </c>
+      <c r="P97" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/amsterdam_annex_gem</t>
-        </is>
-      </c>
-      <c r="P97" t="inlineStr">
-        <is>
-          <t>https://archief.amsterdam/uitleg/indexen/67-bevolkingsregister-geannexeerde-gemeenten-1830-1921</t>
         </is>
       </c>
     </row>
@@ -6451,12 +6451,12 @@
       </c>
       <c r="O98" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P98" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/fak_noat</t>
-        </is>
-      </c>
-      <c r="P98" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -6513,12 +6513,12 @@
       </c>
       <c r="O99" t="inlineStr">
         <is>
+          <t>https://www.archiefeemland.nl/</t>
+        </is>
+      </c>
+      <c r="P99" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/status/closed/project/gam2</t>
-        </is>
-      </c>
-      <c r="P99" t="inlineStr">
-        <is>
-          <t>https://www.archiefeemland.nl/</t>
         </is>
       </c>
     </row>
@@ -6575,12 +6575,12 @@
       </c>
       <c r="O100" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P100" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/status/closed/project/utr_bvr</t>
-        </is>
-      </c>
-      <c r="P100" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -6637,12 +6637,12 @@
       </c>
       <c r="O101" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P101" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/glv_reuvens_transkribus</t>
-        </is>
-      </c>
-      <c r="P101" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -6697,12 +6697,12 @@
       </c>
       <c r="O102" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P102" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/gea_tagging</t>
-        </is>
-      </c>
-      <c r="P102" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -6757,12 +6757,12 @@
       </c>
       <c r="O103" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P103" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/moei_index_30dagen</t>
-        </is>
-      </c>
-      <c r="P103" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -6819,12 +6819,12 @@
       </c>
       <c r="O104" t="inlineStr">
         <is>
+          <t>https://hisgis.nl/projecten/drenthe/</t>
+        </is>
+      </c>
+      <c r="P104" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/2/project/fak_oat</t>
-        </is>
-      </c>
-      <c r="P104" t="inlineStr">
-        <is>
-          <t>https://hisgis.nl/projecten/drenthe/</t>
         </is>
       </c>
     </row>
@@ -6881,12 +6881,12 @@
       </c>
       <c r="O105" t="inlineStr">
         <is>
+          <t>https://www.archiefeemland.nl/</t>
+        </is>
+      </c>
+      <c r="P105" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/3/project/gam</t>
-        </is>
-      </c>
-      <c r="P105" t="inlineStr">
-        <is>
-          <t>https://www.archiefeemland.nl/</t>
         </is>
       </c>
     </row>
@@ -6943,12 +6943,12 @@
       </c>
       <c r="O106" t="inlineStr">
         <is>
+          <t>https://hetutrechtsarchief.nl/onderzoek/resultaten/archieven?mivast=39&amp;mizig=210&amp;miadt=39&amp;miaet=1&amp;micode=1007-2&amp;minr=1307084&amp;miview=inv2&amp;milang=nl</t>
+        </is>
+      </c>
+      <c r="P106" t="inlineStr">
+        <is>
           <t>https://utrecht.nieuws.nl/onderwijswetenschap/74887/utrechts-archief-vraagt-hulp-bij-het-ontsluiten-van-utrechtse-bevolkingsregisters/</t>
-        </is>
-      </c>
-      <c r="P106" t="inlineStr">
-        <is>
-          <t>https://hetutrechtsarchief.nl/onderzoek/resultaten/archieven?mivast=39&amp;mizig=210&amp;miadt=39&amp;miaet=1&amp;micode=1007-2&amp;minr=1307084&amp;miview=inv2&amp;milang=nl</t>
         </is>
       </c>
     </row>
@@ -7005,12 +7005,12 @@
       </c>
       <c r="O107" t="inlineStr">
         <is>
+          <t>https://archief.ajax.nl/</t>
+        </is>
+      </c>
+      <c r="P107" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/2/project/afc_tagging</t>
-        </is>
-      </c>
-      <c r="P107" t="inlineStr">
-        <is>
-          <t>https://archief.ajax.nl/</t>
         </is>
       </c>
     </row>
@@ -7065,12 +7065,12 @@
       </c>
       <c r="O108" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P108" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/amsterdam_notarieel_2</t>
-        </is>
-      </c>
-      <c r="P108" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -7127,12 +7127,12 @@
       </c>
       <c r="O109" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P109" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/status/closed/project/rivierenland_bvr</t>
-        </is>
-      </c>
-      <c r="P109" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -7189,12 +7189,12 @@
       </c>
       <c r="O110" t="inlineStr">
         <is>
+          <t>http://alledrenten.nl/</t>
+        </is>
+      </c>
+      <c r="P110" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/2/project/dre_cmw</t>
-        </is>
-      </c>
-      <c r="P110" t="inlineStr">
-        <is>
-          <t>http://alledrenten.nl/</t>
         </is>
       </c>
     </row>
@@ -7249,12 +7249,12 @@
       </c>
       <c r="O111" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P111" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/hco_resoluties_transkribus</t>
-        </is>
-      </c>
-      <c r="P111" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -7311,12 +7311,12 @@
       </c>
       <c r="O112" t="inlineStr">
         <is>
+          <t>https://stadsarchief.breda.nl/collectie/archief/genealogische-bronnen/persons</t>
+        </is>
+      </c>
+      <c r="P112" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/brd</t>
-        </is>
-      </c>
-      <c r="P112" t="inlineStr">
-        <is>
-          <t>https://stadsarchief.breda.nl/collectie/archief/genealogische-bronnen/persons</t>
         </is>
       </c>
     </row>
@@ -7373,12 +7373,12 @@
       </c>
       <c r="O113" t="inlineStr">
         <is>
+          <t>https://www.erfgoedleiden.nl/collecties/personen</t>
+        </is>
+      </c>
+      <c r="P113" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/leiden</t>
-        </is>
-      </c>
-      <c r="P113" t="inlineStr">
-        <is>
-          <t>https://www.erfgoedleiden.nl/collecties/personen</t>
         </is>
       </c>
     </row>
@@ -7435,12 +7435,12 @@
       </c>
       <c r="O114" t="inlineStr">
         <is>
+          <t>https://www.westfriesarchief.nl/</t>
+        </is>
+      </c>
+      <c r="P114" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/2/project/wfg</t>
-        </is>
-      </c>
-      <c r="P114" t="inlineStr">
-        <is>
-          <t>https://www.westfriesarchief.nl/</t>
         </is>
       </c>
     </row>
@@ -7495,12 +7495,12 @@
       </c>
       <c r="O115" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P115" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/sibr_annotate</t>
-        </is>
-      </c>
-      <c r="P115" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -7557,12 +7557,12 @@
       </c>
       <c r="O116" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P116" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/status/closed/project/picvh_vpr</t>
-        </is>
-      </c>
-      <c r="P116" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -7619,12 +7619,12 @@
       </c>
       <c r="O117" t="inlineStr">
         <is>
+          <t>https://literatuurmuseum.nl/</t>
+        </is>
+      </c>
+      <c r="P117" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/lkm_index</t>
-        </is>
-      </c>
-      <c r="P117" t="inlineStr">
-        <is>
-          <t>https://literatuurmuseum.nl/</t>
         </is>
       </c>
     </row>
@@ -7681,12 +7681,12 @@
       </c>
       <c r="O118" t="inlineStr">
         <is>
+          <t>https://erfgoedcentrumzutphen.nl/onderzoeken/archieven/details/NL-ZuRAZ-0110/path/2.4.1.2.19</t>
+        </is>
+      </c>
+      <c r="P118" t="inlineStr">
+        <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/2/project/szu_bevolkingsregister</t>
-        </is>
-      </c>
-      <c r="P118" t="inlineStr">
-        <is>
-          <t>https://erfgoedcentrumzutphen.nl/onderzoeken/archieven/details/NL-ZuRAZ-0110/path/2.4.1.2.19</t>
         </is>
       </c>
     </row>
@@ -7741,12 +7741,12 @@
       </c>
       <c r="O119" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P119" t="inlineStr">
+        <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/airsenseur</t>
-        </is>
-      </c>
-      <c r="P119" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -7805,12 +7805,12 @@
       </c>
       <c r="O120" t="inlineStr">
         <is>
+          <t>https://login.munisense.net/login?url=https%3A%2F%2Foutdoorclimate.munisense.net%2F&amp;theme=munisense-v2-lhis</t>
+        </is>
+      </c>
+      <c r="P120" t="inlineStr">
+        <is>
           <t>https://inhillegersberg.nl/geluid-lucht/424-luchtmeetnet-hillegersberg-schiebroek</t>
-        </is>
-      </c>
-      <c r="P120" t="inlineStr">
-        <is>
-          <t>https://login.munisense.net/login?url=https%3A%2F%2Foutdoorclimate.munisense.net%2F&amp;theme=munisense-v2-lhis</t>
         </is>
       </c>
     </row>
@@ -7867,12 +7867,12 @@
       </c>
       <c r="O121" t="inlineStr">
         <is>
+          <t>https://samenmeten.rivm.nl/vuurwerk/</t>
+        </is>
+      </c>
+      <c r="P121" t="inlineStr">
+        <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/projecten/vuurwerkexperiment-2019-2020</t>
-        </is>
-      </c>
-      <c r="P121" t="inlineStr">
-        <is>
-          <t>https://samenmeten.rivm.nl/vuurwerk/</t>
         </is>
       </c>
     </row>
@@ -7927,12 +7927,12 @@
       </c>
       <c r="O122" t="inlineStr">
         <is>
+          <t>https://watermonsters.natuurenmilieu.nl/kaart</t>
+        </is>
+      </c>
+      <c r="P122" t="inlineStr">
+        <is>
           <t>https://www.natuurenmilieu.nl/themas/voedsel/projecten-voedsel/waterkwaliteit-biodiversiteit/watermonsters/</t>
-        </is>
-      </c>
-      <c r="P122" t="inlineStr">
-        <is>
-          <t>https://watermonsters.natuurenmilieu.nl/kaart</t>
         </is>
       </c>
     </row>
@@ -7991,12 +7991,12 @@
       </c>
       <c r="O123" t="inlineStr">
         <is>
+          <t>https://samenmeten.rivm.nl/dataportaal/</t>
+        </is>
+      </c>
+      <c r="P123" t="inlineStr">
+        <is>
           <t>http://behouddeparel.nl/samen-meten</t>
-        </is>
-      </c>
-      <c r="P123" t="inlineStr">
-        <is>
-          <t>https://samenmeten.rivm.nl/dataportaal/</t>
         </is>
       </c>
     </row>
@@ -8051,12 +8051,12 @@
       </c>
       <c r="O124" t="inlineStr">
         <is>
+          <t>https://vis.globe.gov/GLOBE/</t>
+        </is>
+      </c>
+      <c r="P124" t="inlineStr">
+        <is>
           <t>https://globenederland.nl/onderzoeksproject/weer/#info</t>
-        </is>
-      </c>
-      <c r="P124" t="inlineStr">
-        <is>
-          <t>https://vis.globe.gov/GLOBE/</t>
         </is>
       </c>
     </row>
@@ -8119,12 +8119,12 @@
       </c>
       <c r="O125" t="inlineStr">
         <is>
+          <t>https://www.tudelft.nl/scd/waterlab/doe-mee-aan-onderzoek/onderzoeksresultaten</t>
+        </is>
+      </c>
+      <c r="P125" t="inlineStr">
+        <is>
           <t>https://www.tudelft.nl/scd/waterlab/doe-mee-aan-onderzoek/project-7-delft-meet-regen</t>
-        </is>
-      </c>
-      <c r="P125" t="inlineStr">
-        <is>
-          <t>https://www.tudelft.nl/scd/waterlab/doe-mee-aan-onderzoek/onderzoeksresultaten</t>
         </is>
       </c>
     </row>
@@ -8183,12 +8183,12 @@
       </c>
       <c r="O126" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P126" t="inlineStr">
+        <is>
           <t>https://www.naturalis.nl/collectie/verborgen-vlinders-het-gestroomlijnd-zichtbaar-maken-van-papillotten</t>
-        </is>
-      </c>
-      <c r="P126" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -8249,12 +8249,12 @@
       </c>
       <c r="O127" t="inlineStr">
         <is>
+          <t>https://milieudefensie.nl/actueel/rapport-wat-adem-jij-in.pdf</t>
+        </is>
+      </c>
+      <c r="P127" t="inlineStr">
+        <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/projecten/meetcampagne-no2-milieudefensie</t>
-        </is>
-      </c>
-      <c r="P127" t="inlineStr">
-        <is>
-          <t>https://milieudefensie.nl/actueel/rapport-wat-adem-jij-in.pdf</t>
         </is>
       </c>
     </row>
@@ -8313,12 +8313,12 @@
       </c>
       <c r="O128" t="inlineStr">
         <is>
+          <t>https://samenmeten.rivm.nl/dataportaal/</t>
+        </is>
+      </c>
+      <c r="P128" t="inlineStr">
+        <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/maaspoort-meet</t>
-        </is>
-      </c>
-      <c r="P128" t="inlineStr">
-        <is>
-          <t>https://samenmeten.rivm.nl/dataportaal/</t>
         </is>
       </c>
     </row>
@@ -8379,12 +8379,12 @@
       </c>
       <c r="O129" t="inlineStr">
         <is>
+          <t>https://amt.copernicus.org/articles/11/1297/2018/</t>
+        </is>
+      </c>
+      <c r="P129" t="inlineStr">
+        <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/projecten/urban-airq-amsterdam</t>
-        </is>
-      </c>
-      <c r="P129" t="inlineStr">
-        <is>
-          <t>https://amt.copernicus.org/articles/11/1297/2018/</t>
         </is>
       </c>
     </row>
@@ -8443,12 +8443,12 @@
       </c>
       <c r="O130" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P130" t="inlineStr">
+        <is>
           <t>https://www.tudelft.nl/scd/waterlab/doe-mee-aan-onderzoek/project-4-oeverwatch</t>
-        </is>
-      </c>
-      <c r="P130" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -8503,12 +8503,12 @@
       </c>
       <c r="O131" t="inlineStr">
         <is>
+          <t>https://grafana.sensemakersams.org/d/m2HAkciWk/mijn-omgeving?orgId=1</t>
+        </is>
+      </c>
+      <c r="P131" t="inlineStr">
+        <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/projecten/watermetingen-door-mijn-omgeving</t>
-        </is>
-      </c>
-      <c r="P131" t="inlineStr">
-        <is>
-          <t>https://grafana.sensemakersams.org/d/m2HAkciWk/mijn-omgeving?orgId=1</t>
         </is>
       </c>
     </row>
@@ -8567,12 +8567,12 @@
       </c>
       <c r="O132" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P132" t="inlineStr">
+        <is>
           <t>https://www.flevoland.nl/dossiers/waterlab-circulair-water</t>
-        </is>
-      </c>
-      <c r="P132" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -8633,12 +8633,12 @@
       </c>
       <c r="O133" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P133" t="inlineStr">
+        <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/visibilis</t>
-        </is>
-      </c>
-      <c r="P133" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -8693,12 +8693,12 @@
       </c>
       <c r="O134" t="inlineStr">
         <is>
+          <t>http://maps.bodemdata.nl/bodemdatanl/index.jsp</t>
+        </is>
+      </c>
+      <c r="P134" t="inlineStr">
+        <is>
           <t>https://globenederland.nl/onderzoeksproject/bodem/#metingen</t>
-        </is>
-      </c>
-      <c r="P134" t="inlineStr">
-        <is>
-          <t>http://maps.bodemdata.nl/bodemdatanl/index.jsp</t>
         </is>
       </c>
     </row>
@@ -8753,12 +8753,12 @@
       </c>
       <c r="O135" t="inlineStr">
         <is>
+          <t>https://wsrivierenland.maps.arcgis.com/apps/MapSeries/index.html?appid=ecdc63fe87bc431db608377635fa2567</t>
+        </is>
+      </c>
+      <c r="P135" t="inlineStr">
+        <is>
           <t>http://altena.gripopwater.nl/over-ons/</t>
-        </is>
-      </c>
-      <c r="P135" t="inlineStr">
-        <is>
-          <t>https://wsrivierenland.maps.arcgis.com/apps/MapSeries/index.html?appid=ecdc63fe87bc431db608377635fa2567</t>
         </is>
       </c>
     </row>
@@ -8817,12 +8817,12 @@
       </c>
       <c r="O136" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P136" t="inlineStr">
+        <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/metingen-s-gravendijkwal-rotterdam</t>
-        </is>
-      </c>
-      <c r="P136" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -8881,12 +8881,12 @@
       </c>
       <c r="O137" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P137" t="inlineStr">
+        <is>
           <t>https://boerenmetenwater.nl/aanleiding/</t>
-        </is>
-      </c>
-      <c r="P137" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -8941,12 +8941,12 @@
       </c>
       <c r="O138" t="inlineStr">
         <is>
+          <t xml:space="preserve">https://samenmeten.rivm.nl/dataportaal/ </t>
+        </is>
+      </c>
+      <c r="P138" t="inlineStr">
+        <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/projecten/samen-stikstofdioxide-meten-met-Palmes-buisjes</t>
-        </is>
-      </c>
-      <c r="P138" t="inlineStr">
-        <is>
-          <t xml:space="preserve">https://samenmeten.rivm.nl/dataportaal/ </t>
         </is>
       </c>
     </row>
@@ -9069,12 +9069,12 @@
       </c>
       <c r="O140" t="inlineStr">
         <is>
+          <t>https://www.arcgis.com/home/webmap/viewer.html?webmap=3eb9b39fda224e1086ce8b8ffdacf053&amp;extent=6.0562,53.4204,6.2258,53.4812</t>
+        </is>
+      </c>
+      <c r="P140" t="inlineStr">
+        <is>
           <t>https://survey123.arcgis.com/share/9c12036c270940c58de97252e1676ea8</t>
-        </is>
-      </c>
-      <c r="P140" t="inlineStr">
-        <is>
-          <t>https://www.arcgis.com/home/webmap/viewer.html?webmap=3eb9b39fda224e1086ce8b8ffdacf053&amp;extent=6.0562,53.4204,6.2258,53.4812</t>
         </is>
       </c>
     </row>
@@ -9133,12 +9133,12 @@
       </c>
       <c r="O141" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P141" t="inlineStr">
+        <is>
           <t>https://www.tudelft.nl/scd/waterlab/doe-mee-aan-onderzoek/project-5-zet-m-op-70</t>
-        </is>
-      </c>
-      <c r="P141" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -9197,12 +9197,12 @@
       </c>
       <c r="O142" t="inlineStr">
         <is>
+          <t>https://hollandseluchten.waag.org/kaart/</t>
+        </is>
+      </c>
+      <c r="P142" t="inlineStr">
+        <is>
           <t>https://hollandseluchten.waag.org/</t>
-        </is>
-      </c>
-      <c r="P142" t="inlineStr">
-        <is>
-          <t>https://hollandseluchten.waag.org/kaart/</t>
         </is>
       </c>
     </row>
@@ -9257,12 +9257,12 @@
       </c>
       <c r="O143" t="inlineStr">
         <is>
+          <t>https://www.tudelft.nl/scd/waterlab/doe-mee-aan-onderzoek/onderzoeksresultaten</t>
+        </is>
+      </c>
+      <c r="P143" t="inlineStr">
+        <is>
           <t>https://drinkablerivers.org/what-we-do/citizen-science/</t>
-        </is>
-      </c>
-      <c r="P143" t="inlineStr">
-        <is>
-          <t>https://www.tudelft.nl/scd/waterlab/doe-mee-aan-onderzoek/onderzoeksresultaten</t>
         </is>
       </c>
     </row>
@@ -9319,12 +9319,12 @@
       </c>
       <c r="O144" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P144" t="inlineStr">
+        <is>
           <t>https://globenederland.nl/onderzoeksprojecten/lichtmeting/</t>
-        </is>
-      </c>
-      <c r="P144" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -9383,12 +9383,12 @@
       </c>
       <c r="O145" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P145" t="inlineStr">
+        <is>
           <t>https://www.scorewater.eu/#3cases</t>
-        </is>
-      </c>
-      <c r="P145" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -9451,12 +9451,12 @@
       </c>
       <c r="O146" t="inlineStr">
         <is>
+          <t>https://snuffelfiets.nl/data/</t>
+        </is>
+      </c>
+      <c r="P146" t="inlineStr">
+        <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/snuffelfiets</t>
-        </is>
-      </c>
-      <c r="P146" t="inlineStr">
-        <is>
-          <t>https://snuffelfiets.nl/data/</t>
         </is>
       </c>
     </row>
@@ -9515,12 +9515,12 @@
       </c>
       <c r="O147" t="inlineStr">
         <is>
+          <t>https://www.eyeonwater.org/search/</t>
+        </is>
+      </c>
+      <c r="P147" t="inlineStr">
+        <is>
           <t>https://www.eyeonwater.org/about-us</t>
-        </is>
-      </c>
-      <c r="P147" t="inlineStr">
-        <is>
-          <t>https://www.eyeonwater.org/search/</t>
         </is>
       </c>
     </row>
@@ -9579,12 +9579,12 @@
       </c>
       <c r="O148" t="inlineStr">
         <is>
+          <t>https://amsterdamsounds.waag.org/kaart/</t>
+        </is>
+      </c>
+      <c r="P148" t="inlineStr">
+        <is>
           <t>https://amsterdamsounds.waag.org/</t>
-        </is>
-      </c>
-      <c r="P148" t="inlineStr">
-        <is>
-          <t>https://amsterdamsounds.waag.org/kaart/</t>
         </is>
       </c>
     </row>
@@ -9639,12 +9639,12 @@
       </c>
       <c r="O149" t="inlineStr">
         <is>
+          <t>https://reports.explane.org/nl/</t>
+        </is>
+      </c>
+      <c r="P149" t="inlineStr">
+        <is>
           <t>https://explane.org/#:~:text=ExPlane%20is%20the%20app%20to%20register%20aviation%20noise&amp;text=The%20app%20gives%20you%20the,by%20residents%20living%20near%20airports</t>
-        </is>
-      </c>
-      <c r="P149" t="inlineStr">
-        <is>
-          <t>https://reports.explane.org/nl/</t>
         </is>
       </c>
     </row>
@@ -9699,12 +9699,12 @@
       </c>
       <c r="O150" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P150" t="inlineStr">
+        <is>
           <t>https://www.tudelft.nl/scd/waterlab/doe-mee-aan-onderzoek/project-2-check-de-stadsvergroening</t>
-        </is>
-      </c>
-      <c r="P150" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -9763,12 +9763,12 @@
       </c>
       <c r="O151" t="inlineStr">
         <is>
+          <t xml:space="preserve">https://samenmeten.rivm.nl/dataportaal/  </t>
+        </is>
+      </c>
+      <c r="P151" t="inlineStr">
+        <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/projecten/samen-luchtkwaliteit-meten-in-zuid-holland</t>
-        </is>
-      </c>
-      <c r="P151" t="inlineStr">
-        <is>
-          <t xml:space="preserve">https://samenmeten.rivm.nl/dataportaal/  </t>
         </is>
       </c>
     </row>
@@ -9831,12 +9831,12 @@
       </c>
       <c r="O152" t="inlineStr">
         <is>
+          <t>https://samenmeten.rivm.nl/dataportaal/</t>
+        </is>
+      </c>
+      <c r="P152" t="inlineStr">
+        <is>
           <t xml:space="preserve">https://www.samenmetenaanluchtkwaliteit.nl/projecten/samen-houtrook-meten </t>
-        </is>
-      </c>
-      <c r="P152" t="inlineStr">
-        <is>
-          <t>https://samenmeten.rivm.nl/dataportaal/</t>
         </is>
       </c>
     </row>
@@ -9893,12 +9893,12 @@
       </c>
       <c r="O153" t="inlineStr">
         <is>
+          <t>https://samenmeten.rivm.nl/dataportaal/</t>
+        </is>
+      </c>
+      <c r="P153" t="inlineStr">
+        <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/vuurwerkexperiment-2018-2019</t>
-        </is>
-      </c>
-      <c r="P153" t="inlineStr">
-        <is>
-          <t>https://samenmeten.rivm.nl/dataportaal/</t>
         </is>
       </c>
     </row>
@@ -9959,12 +9959,12 @@
       </c>
       <c r="O154" t="inlineStr">
         <is>
+          <t>https://almeremeetwater.nl/kaart/</t>
+        </is>
+      </c>
+      <c r="P154" t="inlineStr">
+        <is>
           <t>https://almeremeetwater.nl/</t>
-        </is>
-      </c>
-      <c r="P154" t="inlineStr">
-        <is>
-          <t>https://almeremeetwater.nl/kaart/</t>
         </is>
       </c>
     </row>
@@ -10021,12 +10021,12 @@
       </c>
       <c r="O155" t="inlineStr">
         <is>
+          <t>https://www.arcgis.com/home/webmap/viewer.html?webmap=9f6c2e258f2f40a884335feaf85501a7&amp;extent=3.9538,51.8158,4.968,52.1811</t>
+        </is>
+      </c>
+      <c r="P155" t="inlineStr">
+        <is>
           <t>https://www.tudelft.nl/scd/waterlab/doe-mee-aan-onderzoek/project-1-waterkwaliteit-in-europa</t>
-        </is>
-      </c>
-      <c r="P155" t="inlineStr">
-        <is>
-          <t>https://www.arcgis.com/home/webmap/viewer.html?webmap=9f6c2e258f2f40a884335feaf85501a7&amp;extent=3.9538,51.8158,4.968,52.1811</t>
         </is>
       </c>
     </row>
@@ -10085,12 +10085,12 @@
       </c>
       <c r="O156" t="inlineStr">
         <is>
+          <t>https://data.smartemission.nl/data</t>
+        </is>
+      </c>
+      <c r="P156" t="inlineStr">
+        <is>
           <t>https://data.smartemission.nl/home</t>
-        </is>
-      </c>
-      <c r="P156" t="inlineStr">
-        <is>
-          <t>https://data.smartemission.nl/data</t>
         </is>
       </c>
     </row>
@@ -10149,12 +10149,12 @@
       </c>
       <c r="O157" t="inlineStr">
         <is>
+          <t>https://www.meetjestad.net/data/</t>
+        </is>
+      </c>
+      <c r="P157" t="inlineStr">
+        <is>
           <t>https://www.meetjestad.net/nl/MeetjeStad</t>
-        </is>
-      </c>
-      <c r="P157" t="inlineStr">
-        <is>
-          <t>https://www.meetjestad.net/data/</t>
         </is>
       </c>
     </row>
@@ -10211,12 +10211,12 @@
       </c>
       <c r="O158" t="inlineStr">
         <is>
+          <t>https://samenmeten.rivm.nl/dataportaal/</t>
+        </is>
+      </c>
+      <c r="P158" t="inlineStr">
+        <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/vuurwerkexperiment-20172018</t>
-        </is>
-      </c>
-      <c r="P158" t="inlineStr">
-        <is>
-          <t>https://samenmeten.rivm.nl/dataportaal/</t>
         </is>
       </c>
     </row>
@@ -10273,12 +10273,12 @@
       </c>
       <c r="O159" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P159" t="inlineStr">
+        <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/ispex</t>
-        </is>
-      </c>
-      <c r="P159" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -10337,12 +10337,12 @@
       </c>
       <c r="O160" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P160" t="inlineStr">
+        <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/aireas-eindhoven</t>
-        </is>
-      </c>
-      <c r="P160" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -10399,12 +10399,12 @@
       </c>
       <c r="O161" t="inlineStr">
         <is>
+          <t>https://samenmeten.rivm.nl/vuurwerk/</t>
+        </is>
+      </c>
+      <c r="P161" t="inlineStr">
+        <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/oud-nieuw-2020-2021</t>
-        </is>
-      </c>
-      <c r="P161" t="inlineStr">
-        <is>
-          <t>https://samenmeten.rivm.nl/vuurwerk/</t>
         </is>
       </c>
     </row>
@@ -10459,12 +10459,12 @@
       </c>
       <c r="O162" t="inlineStr">
         <is>
+          <t>https://samenmeten.rivm.nl/dataportaal/</t>
+        </is>
+      </c>
+      <c r="P162" t="inlineStr">
+        <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/</t>
-        </is>
-      </c>
-      <c r="P162" t="inlineStr">
-        <is>
-          <t>https://samenmeten.rivm.nl/dataportaal/</t>
         </is>
       </c>
     </row>
@@ -10521,12 +10521,12 @@
       </c>
       <c r="O163" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P163" t="inlineStr">
+        <is>
           <t>https://www.kwrwater.nl/projecten/citizen-science-praktijkpilot-versheid-water/</t>
-        </is>
-      </c>
-      <c r="P163" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -10583,12 +10583,12 @@
       </c>
       <c r="O164" t="inlineStr">
         <is>
+          <t xml:space="preserve">https://samenmeten.rivm.nl/dataportaal/  </t>
+        </is>
+      </c>
+      <c r="P164" t="inlineStr">
+        <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/vuurwerk-2016-2017</t>
-        </is>
-      </c>
-      <c r="P164" t="inlineStr">
-        <is>
-          <t xml:space="preserve">https://samenmeten.rivm.nl/dataportaal/  </t>
         </is>
       </c>
     </row>
@@ -10643,12 +10643,12 @@
       </c>
       <c r="O165" t="inlineStr">
         <is>
+          <t>https://samenmeten.rivm.nl/dataportaal/</t>
+        </is>
+      </c>
+      <c r="P165" t="inlineStr">
+        <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/luftdaten</t>
-        </is>
-      </c>
-      <c r="P165" t="inlineStr">
-        <is>
-          <t>https://samenmeten.rivm.nl/dataportaal/</t>
         </is>
       </c>
     </row>
@@ -10707,12 +10707,12 @@
       </c>
       <c r="O166" t="inlineStr">
         <is>
+          <t>https://www.webgispublisher.nl/schiedam/</t>
+        </is>
+      </c>
+      <c r="P166" t="inlineStr">
+        <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/burgermetingen-schiedam</t>
-        </is>
-      </c>
-      <c r="P166" t="inlineStr">
-        <is>
-          <t>https://www.webgispublisher.nl/schiedam/</t>
         </is>
       </c>
     </row>
@@ -10773,12 +10773,12 @@
       </c>
       <c r="O167" t="inlineStr">
         <is>
+          <t xml:space="preserve">https://samenmeten.rivm.nl/dataportaal/ </t>
+        </is>
+      </c>
+      <c r="P167" t="inlineStr">
+        <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/jubileumproject-dcmr-no2-burgermetingen-in-rijnmondgebied</t>
-        </is>
-      </c>
-      <c r="P167" t="inlineStr">
-        <is>
-          <t xml:space="preserve">https://samenmeten.rivm.nl/dataportaal/ </t>
         </is>
       </c>
     </row>
@@ -10839,12 +10839,12 @@
       </c>
       <c r="O168" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P168" t="inlineStr">
+        <is>
           <t>https://www.waterforum.net/officiele-start-waterlab-flevoland/</t>
-        </is>
-      </c>
-      <c r="P168" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -10899,12 +10899,12 @@
       </c>
       <c r="O169" t="inlineStr">
         <is>
+          <t>https://samenmeten.rivm.nl/dataportaal/</t>
+        </is>
+      </c>
+      <c r="P169" t="inlineStr">
+        <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/projecten/onze-lucht-zelf-fijnstof-meten-in-noord-nederland</t>
-        </is>
-      </c>
-      <c r="P169" t="inlineStr">
-        <is>
-          <t>https://samenmeten.rivm.nl/dataportaal/</t>
         </is>
       </c>
     </row>
@@ -10959,12 +10959,12 @@
       </c>
       <c r="O170" t="inlineStr">
         <is>
+          <t>https://www.schonerivieren.org/join/resultaten-onderzoeken/</t>
+        </is>
+      </c>
+      <c r="P170" t="inlineStr">
+        <is>
           <t>https://www.iedereenwetenschapper.be/projects/word-afvalonderzoeker</t>
-        </is>
-      </c>
-      <c r="P170" t="inlineStr">
-        <is>
-          <t>https://www.schonerivieren.org/join/resultaten-onderzoeken/</t>
         </is>
       </c>
     </row>
@@ -11089,12 +11089,12 @@
       </c>
       <c r="O172" t="inlineStr">
         <is>
+          <t>https://www.luchtmeetnet-maastricht.nl/maastricht/</t>
+        </is>
+      </c>
+      <c r="P172" t="inlineStr">
+        <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/maastricht</t>
-        </is>
-      </c>
-      <c r="P172" t="inlineStr">
-        <is>
-          <t>https://www.luchtmeetnet-maastricht.nl/maastricht/</t>
         </is>
       </c>
     </row>
@@ -11149,12 +11149,12 @@
       </c>
       <c r="O173" t="inlineStr">
         <is>
+          <t>https://samenmeten.rivm.nl/dataportaal/</t>
+        </is>
+      </c>
+      <c r="P173" t="inlineStr">
+        <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/projecten/samen-geluid-meten</t>
-        </is>
-      </c>
-      <c r="P173" t="inlineStr">
-        <is>
-          <t>https://samenmeten.rivm.nl/dataportaal/</t>
         </is>
       </c>
     </row>
@@ -11215,12 +11215,12 @@
       </c>
       <c r="O174" t="inlineStr">
         <is>
+          <t>https://samenmeten.rivm.nl/dataportaal/</t>
+        </is>
+      </c>
+      <c r="P174" t="inlineStr">
+        <is>
           <t>https://www.rivm.nl/boeren-en-buren</t>
-        </is>
-      </c>
-      <c r="P174" t="inlineStr">
-        <is>
-          <t>https://samenmeten.rivm.nl/dataportaal/</t>
         </is>
       </c>
     </row>
@@ -11275,12 +11275,12 @@
       </c>
       <c r="O175" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P175" t="inlineStr">
+        <is>
           <t>https://www.tuintelling.nl/index.php/data/result/evenement/ES/</t>
-        </is>
-      </c>
-      <c r="P175" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -11341,12 +11341,12 @@
       </c>
       <c r="O176" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P176" t="inlineStr">
+        <is>
           <t>https://www.universiteitleiden.nl/citizensciencelab/projecten/oeverplanten</t>
-        </is>
-      </c>
-      <c r="P176" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -11401,12 +11401,12 @@
       </c>
       <c r="O177" t="inlineStr">
         <is>
+          <t>https://www.nioz.nl/en/about/cos/movement-connectivity/bird-movement/tracking-movements-of-spoonbills/follow-spoonbills-from-the-netherlands</t>
+        </is>
+      </c>
+      <c r="P177" t="inlineStr">
+        <is>
           <t>https://www.iedereenwetenschapper.be/projects/volg-de-weg-van-trekvogels</t>
-        </is>
-      </c>
-      <c r="P177" t="inlineStr">
-        <is>
-          <t>https://www.nioz.nl/en/about/cos/movement-connectivity/bird-movement/tracking-movements-of-spoonbills/follow-spoonbills-from-the-netherlands</t>
         </is>
       </c>
     </row>
@@ -11461,12 +11461,12 @@
       </c>
       <c r="O178" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P178" t="inlineStr">
+        <is>
           <t>https://www.tuintelling.nl/data/result/evenement/EPLONS</t>
-        </is>
-      </c>
-      <c r="P178" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -11521,12 +11521,12 @@
       </c>
       <c r="O179" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P179" t="inlineStr">
+        <is>
           <t>https://www.naturetoday.com/intl/nl/nature-reports/message/?msg=27308</t>
-        </is>
-      </c>
-      <c r="P179" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -11581,12 +11581,12 @@
       </c>
       <c r="O180" t="inlineStr">
         <is>
+          <t>https://euring.org/data-and-codes/obtaining-data</t>
+        </is>
+      </c>
+      <c r="P180" t="inlineStr">
+        <is>
           <t>https://vogeltrekstation.nl/nl/onderzoek/monitoringsprojecten/zo%C3%B6nosenproject</t>
-        </is>
-      </c>
-      <c r="P180" t="inlineStr">
-        <is>
-          <t>https://euring.org/data-and-codes/obtaining-data</t>
         </is>
       </c>
     </row>
@@ -11643,12 +11643,12 @@
       </c>
       <c r="O181" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P181" t="inlineStr">
+        <is>
           <t>https://www.eis-nederland.nl/wantsenproject</t>
-        </is>
-      </c>
-      <c r="P181" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -11703,12 +11703,12 @@
       </c>
       <c r="O182" t="inlineStr">
         <is>
+          <t>https://www.clo.nl/indicatoren/nl1387-libellen</t>
+        </is>
+      </c>
+      <c r="P182" t="inlineStr">
+        <is>
           <t>https://www.tuintelling.nl/evenementen/libellentelling</t>
-        </is>
-      </c>
-      <c r="P182" t="inlineStr">
-        <is>
-          <t>https://www.clo.nl/indicatoren/nl1387-libellen</t>
         </is>
       </c>
     </row>
@@ -11829,12 +11829,12 @@
       </c>
       <c r="O184" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P184" t="inlineStr">
+        <is>
           <t>https://www.universiteitleiden.nl/citizensciencelab/projecten/evoscope---paardenbloemen</t>
-        </is>
-      </c>
-      <c r="P184" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -11889,12 +11889,12 @@
       </c>
       <c r="O185" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P185" t="inlineStr">
+        <is>
           <t>https://www.floron.nl/meedoen/herbariummateriaal</t>
-        </is>
-      </c>
-      <c r="P185" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -11951,12 +11951,12 @@
       </c>
       <c r="O186" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P186" t="inlineStr">
+        <is>
           <t xml:space="preserve">https://www.tuintelling.nl/evenementen </t>
-        </is>
-      </c>
-      <c r="P186" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -12011,12 +12011,12 @@
       </c>
       <c r="O187" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P187" t="inlineStr">
+        <is>
           <t>https://www.tuintelling.nl/evenementen/kikkerdriltelling</t>
-        </is>
-      </c>
-      <c r="P187" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -12071,12 +12071,12 @@
       </c>
       <c r="O188" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P188" t="inlineStr">
+        <is>
           <t>https://www.hortusleiden.nl/onderwijs/stoepplantjes-1</t>
-        </is>
-      </c>
-      <c r="P188" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -12133,12 +12133,12 @@
       </c>
       <c r="O189" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P189" t="inlineStr">
+        <is>
           <t xml:space="preserve">https://www.tuintelling.nl/evenementen </t>
-        </is>
-      </c>
-      <c r="P189" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -12193,12 +12193,12 @@
       </c>
       <c r="O190" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P190" t="inlineStr">
+        <is>
           <t>https://www.zoogdiervereniging.nl/wat-we-doen/monitoring/jaarrond-tuintelling/mollentelling</t>
-        </is>
-      </c>
-      <c r="P190" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -12253,12 +12253,12 @@
       </c>
       <c r="O191" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P191" t="inlineStr">
+        <is>
           <t>https://www.iedereenwetenschapper.be/projects/bestudeer-wilde-dieren-de-hoge-veluwe</t>
-        </is>
-      </c>
-      <c r="P191" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -12313,12 +12313,12 @@
       </c>
       <c r="O192" t="inlineStr">
         <is>
+          <t>https://euring.org/data-and-codes/obtaining-data</t>
+        </is>
+      </c>
+      <c r="P192" t="inlineStr">
+        <is>
           <t>https://vogeltrekstation.nl/nl/onderzoek/monitoringsprojecten/ces-het-constant-effort-site-project</t>
-        </is>
-      </c>
-      <c r="P192" t="inlineStr">
-        <is>
-          <t>https://euring.org/data-and-codes/obtaining-data</t>
         </is>
       </c>
     </row>
@@ -12373,12 +12373,12 @@
       </c>
       <c r="O193" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P193" t="inlineStr">
+        <is>
           <t>https://www.vogelbescherming.nl/tuinvogeltelling</t>
-        </is>
-      </c>
-      <c r="P193" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -12433,12 +12433,12 @@
       </c>
       <c r="O194" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P194" t="inlineStr">
+        <is>
           <t>https://www.floron.nl/plantenjacht</t>
-        </is>
-      </c>
-      <c r="P194" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -12493,12 +12493,12 @@
       </c>
       <c r="O195" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P195" t="inlineStr">
+        <is>
           <t>https://www.tuintelling.nl/data/result/evenement/EBB</t>
-        </is>
-      </c>
-      <c r="P195" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -12559,12 +12559,12 @@
       </c>
       <c r="O196" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P196" t="inlineStr">
+        <is>
           <t>https://www.naturetoday.com/intl/nl/nature-reports/message/?msg=25068</t>
-        </is>
-      </c>
-      <c r="P196" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -12619,12 +12619,12 @@
       </c>
       <c r="O197" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P197" t="inlineStr">
+        <is>
           <t>https://www.universiteitleiden.nl/citizensciencelab/projecten/naturalis</t>
-        </is>
-      </c>
-      <c r="P197" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -12679,12 +12679,12 @@
       </c>
       <c r="O198" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P198" t="inlineStr">
+        <is>
           <t xml:space="preserve">https://www.floron.nl/meedoen/witte-gebieden </t>
-        </is>
-      </c>
-      <c r="P198" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -12807,12 +12807,12 @@
       </c>
       <c r="O200" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P200" t="inlineStr">
+        <is>
           <t xml:space="preserve">https://www.floron.nl/meedoen/kilometerhokken-inventariseren </t>
-        </is>
-      </c>
-      <c r="P200" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -12867,12 +12867,12 @@
       </c>
       <c r="O201" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P201" t="inlineStr">
+        <is>
           <t>https://www.tuintelling.nl/kraamkamer</t>
-        </is>
-      </c>
-      <c r="P201" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -12931,12 +12931,12 @@
       </c>
       <c r="O202" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P202" t="inlineStr">
+        <is>
           <t>https://www.naturetoday.com/intl/nl/nature-reports/message/?msg=22655</t>
-        </is>
-      </c>
-      <c r="P202" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -12991,12 +12991,12 @@
       </c>
       <c r="O203" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P203" t="inlineStr">
+        <is>
           <t>https://www.tuintelling.nl/data/result/evenement/EE</t>
-        </is>
-      </c>
-      <c r="P203" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -13055,12 +13055,12 @@
       </c>
       <c r="O204" t="inlineStr">
         <is>
+          <t>https://www.growapp.today/#/</t>
+        </is>
+      </c>
+      <c r="P204" t="inlineStr">
+        <is>
           <t>https://www.naturetoday.com/intl/nl/observations/growapp</t>
-        </is>
-      </c>
-      <c r="P204" t="inlineStr">
-        <is>
-          <t>https://www.growapp.today/#/</t>
         </is>
       </c>
     </row>
@@ -13115,12 +13115,12 @@
       </c>
       <c r="O205" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P205" t="inlineStr">
+        <is>
           <t>https://www.vlinderstichting.nl/nachtvlindernacht/</t>
-        </is>
-      </c>
-      <c r="P205" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -13181,12 +13181,12 @@
       </c>
       <c r="O206" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P206" t="inlineStr">
+        <is>
           <t>https://www.tuintelling.nl/evenementen/avondtelling</t>
-        </is>
-      </c>
-      <c r="P206" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -13243,12 +13243,12 @@
       </c>
       <c r="O207" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P207" t="inlineStr">
+        <is>
           <t>https://tuintelling.nl/evenementen/tuinvijvertelling</t>
-        </is>
-      </c>
-      <c r="P207" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -13303,12 +13303,12 @@
       </c>
       <c r="O208" t="inlineStr">
         <is>
+          <t>https://euring.org/data-and-codes/obtaining-data</t>
+        </is>
+      </c>
+      <c r="P208" t="inlineStr">
+        <is>
           <t>https://vogeltrekstation.nl/nl/onderzoek/monitoringsprojecten/pullen#quicktabs-pullen=0</t>
-        </is>
-      </c>
-      <c r="P208" t="inlineStr">
-        <is>
-          <t>https://euring.org/data-and-codes/obtaining-data</t>
         </is>
       </c>
     </row>
@@ -13363,12 +13363,12 @@
       </c>
       <c r="O209" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P209" t="inlineStr">
+        <is>
           <t>https://www.nationalebijentelling.nl/</t>
-        </is>
-      </c>
-      <c r="P209" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -13423,12 +13423,12 @@
       </c>
       <c r="O210" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P210" t="inlineStr">
+        <is>
           <t>https://www.ravon.nl/Portals/2/Bestanden/Publicaties/Rapporten/2007.003k.pdf</t>
-        </is>
-      </c>
-      <c r="P210" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -13483,12 +13483,12 @@
       </c>
       <c r="O211" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P211" t="inlineStr">
+        <is>
           <t>https://www.floron.nl/bermen</t>
-        </is>
-      </c>
-      <c r="P211" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -13543,12 +13543,12 @@
       </c>
       <c r="O212" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P212" t="inlineStr">
+        <is>
           <t>https://www.sovon.nl/nl/actueel/nieuws/lijsters-en-bessen-tellen</t>
-        </is>
-      </c>
-      <c r="P212" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -13603,12 +13603,12 @@
       </c>
       <c r="O213" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P213" t="inlineStr">
+        <is>
           <t>https://www.vleermuis.net/</t>
-        </is>
-      </c>
-      <c r="P213" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -13663,12 +13663,12 @@
       </c>
       <c r="O214" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P214" t="inlineStr">
+        <is>
           <t>https://www.sovon.nl/nl/MUS</t>
-        </is>
-      </c>
-      <c r="P214" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -13723,12 +13723,12 @@
       </c>
       <c r="O215" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P215" t="inlineStr">
+        <is>
           <t>https://submit.cr-birding.org/page/who_are_we/</t>
-        </is>
-      </c>
-      <c r="P215" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -13783,12 +13783,12 @@
       </c>
       <c r="O216" t="inlineStr">
         <is>
+          <t>https://euring.org/data-and-codes/obtaining-data</t>
+        </is>
+      </c>
+      <c r="P216" t="inlineStr">
+        <is>
           <t>https://vogeltrekstation.nl/nl/onderzoek/monitoringsprojecten/boerenzwaluw</t>
-        </is>
-      </c>
-      <c r="P216" t="inlineStr">
-        <is>
-          <t>https://euring.org/data-and-codes/obtaining-data</t>
         </is>
       </c>
     </row>
@@ -13843,12 +13843,12 @@
       </c>
       <c r="O217" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P217" t="inlineStr">
+        <is>
           <t>https://www.naturetoday.com/intl/nl/observations/natuurkalender?utm_source=natuurkalender.nl&amp;utm_medium=redirect&amp;utm_campaign=olddomain</t>
-        </is>
-      </c>
-      <c r="P217" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -13903,12 +13903,12 @@
       </c>
       <c r="O218" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P218" t="inlineStr">
+        <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/projecten/treewifi</t>
-        </is>
-      </c>
-      <c r="P218" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -13965,12 +13965,12 @@
       </c>
       <c r="O219" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P219" t="inlineStr">
+        <is>
           <t>https://www.universiteitleiden.nl/citizensciencelab/projecten/evoscope---kauwtjes</t>
-        </is>
-      </c>
-      <c r="P219" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -14025,12 +14025,12 @@
       </c>
       <c r="O220" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P220" t="inlineStr">
+        <is>
           <t>https://www.naturetoday.com/intl/nl/nature-reports/message/?msg=26207</t>
-        </is>
-      </c>
-      <c r="P220" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -14087,12 +14087,12 @@
       </c>
       <c r="O221" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P221" t="inlineStr">
+        <is>
           <t>https://www.iedereenwetenschapper.be/projects/hoe-gaat-het-met-de-wilde-eend</t>
-        </is>
-      </c>
-      <c r="P221" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -14147,12 +14147,12 @@
       </c>
       <c r="O222" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P222" t="inlineStr">
+        <is>
           <t>https://www.vlinderstichting.nl/vlindermee/</t>
-        </is>
-      </c>
-      <c r="P222" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -14209,12 +14209,12 @@
       </c>
       <c r="O223" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P223" t="inlineStr">
+        <is>
           <t>https://www.universiteitleiden.nl/citizensciencelab/projecten/evoscope---koolmezen</t>
-        </is>
-      </c>
-      <c r="P223" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -14269,12 +14269,12 @@
       </c>
       <c r="O224" t="inlineStr">
         <is>
+          <t>https://euring.org/data-and-codes/obtaining-data</t>
+        </is>
+      </c>
+      <c r="P224" t="inlineStr">
+        <is>
           <t>https://vogeltrekstation.nl/nl/onderzoek/monitoringsprojecten/ras-het-retrapping-adults-survival-project</t>
-        </is>
-      </c>
-      <c r="P224" t="inlineStr">
-        <is>
-          <t>https://euring.org/data-and-codes/obtaining-data</t>
         </is>
       </c>
     </row>
@@ -14331,12 +14331,12 @@
       </c>
       <c r="O225" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P225" t="inlineStr">
+        <is>
           <t>https://www.eis-nederland.nl/actueel/projecten/leuke-vliegen</t>
-        </is>
-      </c>
-      <c r="P225" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -14393,12 +14393,12 @@
       </c>
       <c r="O226" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P226" t="inlineStr">
+        <is>
           <t>https://www.zooniverse.org/projects/anneoverduin/fishing-in-the-past/about/research</t>
-        </is>
-      </c>
-      <c r="P226" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -14453,12 +14453,12 @@
       </c>
       <c r="O227" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P227" t="inlineStr">
+        <is>
           <t>https://www.floron.nl/meedoen/actualisering-groeiplaatsen-bijzondere-soorten</t>
-        </is>
-      </c>
-      <c r="P227" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -14513,12 +14513,12 @@
       </c>
       <c r="O228" t="inlineStr">
         <is>
+          <t>https://www.ndff.nl/overdendff/data/</t>
+        </is>
+      </c>
+      <c r="P228" t="inlineStr">
+        <is>
           <t>https://bodemdierendagen.nl/</t>
-        </is>
-      </c>
-      <c r="P228" t="inlineStr">
-        <is>
-          <t>https://www.ndff.nl/overdendff/data/</t>
         </is>
       </c>
     </row>
@@ -14633,12 +14633,12 @@
       </c>
       <c r="O230" t="inlineStr">
         <is>
+          <t>https://www.cbs.nl/nl-nl/nieuws/2017/01/verspreiding-invasieve-plantensoorten-toegenomen en https://www.clo.nl/indicatoren/nl1398-invasieve-plantensoorten</t>
+        </is>
+      </c>
+      <c r="P230" t="inlineStr">
+        <is>
           <t>https://www.floron.nl/meedoen/exoten-melden</t>
-        </is>
-      </c>
-      <c r="P230" t="inlineStr">
-        <is>
-          <t>https://www.cbs.nl/nl-nl/nieuws/2017/01/verspreiding-invasieve-plantensoorten-toegenomen en https://www.clo.nl/indicatoren/nl1398-invasieve-plantensoorten</t>
         </is>
       </c>
     </row>
@@ -14693,12 +14693,12 @@
       </c>
       <c r="O231" t="inlineStr">
         <is>
+          <t>https://euring.org/data-and-codes/obtaining-data</t>
+        </is>
+      </c>
+      <c r="P231" t="inlineStr">
+        <is>
           <t>https://vogeltrekstation.nl/nl/onderzoek/monitoringsprojecten/ring-mus%20</t>
-        </is>
-      </c>
-      <c r="P231" t="inlineStr">
-        <is>
-          <t>https://euring.org/data-and-codes/obtaining-data</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Apply GitHub Action changes
</commit_message>
<xml_diff>
--- a/data/citizen-science-projects-nl.xlsx
+++ b/data/citizen-science-projects-nl.xlsx
@@ -567,11 +567,7 @@
           <t>Unsure</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/status/closed/project/bhic_strafgevangenissen_2</t>
@@ -629,11 +625,7 @@
           <t>Unsure</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/ja_ik_wil</t>
@@ -689,11 +681,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/tlb_index</t>
@@ -749,11 +737,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/fak_noat</t>
@@ -809,11 +793,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/sibr_annotate</t>
@@ -991,11 +971,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/hga_index_gezinskaarten</t>
@@ -1175,11 +1151,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O12" t="inlineStr"/>
       <c r="P12" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/utr_index_bvr_1850_1889</t>
@@ -1299,11 +1271,7 @@
           <t>Unsure</t>
         </is>
       </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/status/closed/project/utr_bvr</t>
@@ -1421,11 +1389,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/gea_tagging</t>
@@ -1481,11 +1445,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/gra_tagging_vanderveen</t>
@@ -1541,11 +1501,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/huy_correct_resoluties_transkribus</t>
@@ -1725,11 +1681,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/wfg_transcription_notarieel</t>
@@ -1849,11 +1801,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O23" t="inlineStr"/>
       <c r="P23" t="inlineStr">
         <is>
           <t>https://www.iedereenwetenschapper.be/projects/duik-historisch-amsterdam</t>
@@ -1909,11 +1857,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O24" t="inlineStr"/>
       <c r="P24" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/ranh_index</t>
@@ -1969,11 +1913,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O25" t="inlineStr"/>
       <c r="P25" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/vua_train_kronieken_transkribus</t>
@@ -2029,11 +1969,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O26" t="inlineStr"/>
       <c r="P26" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/cbg_index_hal</t>
@@ -2213,11 +2149,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O29" t="inlineStr"/>
       <c r="P29" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/leiden_na1</t>
@@ -2335,11 +2267,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O31" t="inlineStr"/>
       <c r="P31" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/afc_tagging_2</t>
@@ -2459,11 +2387,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O33" t="inlineStr"/>
       <c r="P33" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/picvh_run</t>
@@ -2581,11 +2505,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O35" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O35" t="inlineStr"/>
       <c r="P35" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/wiewaswie_bvr</t>
@@ -2643,11 +2563,7 @@
           <t>Unsure</t>
         </is>
       </c>
-      <c r="O36" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O36" t="inlineStr"/>
       <c r="P36" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/status/closed/project/gda_2</t>
@@ -2701,11 +2617,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O37" t="inlineStr"/>
       <c r="P37" t="inlineStr">
         <is>
           <t>https://www.iedereenwetenschapper.be/projects/reis-terug-de-tijd</t>
@@ -2761,11 +2673,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O38" t="inlineStr"/>
       <c r="P38" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/utrecht_transcription_notarieel</t>
@@ -2823,11 +2731,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O39" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O39" t="inlineStr"/>
       <c r="P39" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/zaa_index_bron</t>
@@ -3005,11 +2909,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O42" t="inlineStr"/>
       <c r="P42" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/moei_index_30dagen</t>
@@ -3375,11 +3275,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O48" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O48" t="inlineStr"/>
       <c r="P48" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/frl</t>
@@ -3621,11 +3517,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O52" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O52" t="inlineStr"/>
       <c r="P52" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/hfl_tagging_rijpcollectie</t>
@@ -3869,11 +3761,7 @@
           <t>Unsure</t>
         </is>
       </c>
-      <c r="O56" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O56" t="inlineStr"/>
       <c r="P56" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/status/closed/project/rivierenland_bvr</t>
@@ -3991,11 +3879,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O58" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O58" t="inlineStr"/>
       <c r="P58" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/bhic_repnot</t>
@@ -4053,11 +3937,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O59" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O59" t="inlineStr"/>
       <c r="P59" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/status/closed/page/1/project/glv_reuvens_transkribus</t>
@@ -4175,11 +4055,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O61" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O61" t="inlineStr"/>
       <c r="P61" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/vua_annoteer_kronieken_transkribus</t>
@@ -4297,11 +4173,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O63" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O63" t="inlineStr"/>
       <c r="P63" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/amsterdam_correct_notarieel_transkribus</t>
@@ -4357,11 +4229,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O64" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O64" t="inlineStr"/>
       <c r="P64" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/gda_index_huwelijk</t>
@@ -4479,11 +4347,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O66" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O66" t="inlineStr"/>
       <c r="P66" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/sahm_index_bevolkingsregisters</t>
@@ -5097,11 +4961,7 @@
           <t>Unsure</t>
         </is>
       </c>
-      <c r="O76" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O76" t="inlineStr"/>
       <c r="P76" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/status/closed/project/picvh_vpr</t>
@@ -5157,11 +5017,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O77" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O77" t="inlineStr"/>
       <c r="P77" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/legermuseum</t>
@@ -5217,11 +5073,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O78" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O78" t="inlineStr"/>
       <c r="P78" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/mei</t>
@@ -5277,11 +5129,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O79" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O79" t="inlineStr"/>
       <c r="P79" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/hco_resoluties_transkribus</t>
@@ -5399,11 +5247,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O81" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O81" t="inlineStr"/>
       <c r="P81" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/rar_index_repertoria</t>
@@ -5459,11 +5303,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O82" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O82" t="inlineStr"/>
       <c r="P82" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/picvh_bhic_bevolkingsregister</t>
@@ -5581,11 +5421,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O84" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O84" t="inlineStr"/>
       <c r="P84" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/amsterdam_notarieel_2</t>
@@ -5641,11 +5477,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O85" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O85" t="inlineStr"/>
       <c r="P85" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/project/zaa_index_gaarder</t>
@@ -5701,11 +5533,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O86" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O86" t="inlineStr"/>
       <c r="P86" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/nfm_tagging_photos</t>
@@ -5823,11 +5651,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O88" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O88" t="inlineStr"/>
       <c r="P88" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/run_slavenregisters</t>
@@ -5945,11 +5769,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O90" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O90" t="inlineStr"/>
       <c r="P90" t="inlineStr">
         <is>
           <t>https://velehanden.nl/projecten/bekijk/details/page/2/project/mai_tagging</t>
@@ -6069,11 +5889,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O92" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O92" t="inlineStr"/>
       <c r="P92" t="inlineStr">
         <is>
           <t>https://www.iedereenwetenschapper.be/projects/download-je-eigen-deeltjesdetector</t>
@@ -6129,11 +5945,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O93" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O93" t="inlineStr"/>
       <c r="P93" t="inlineStr">
         <is>
           <t>https://www.iedereenwetenschapper.be/projects/bekijk-de-aarde-vanuit-de-ruimte</t>
@@ -6251,11 +6063,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O95" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O95" t="inlineStr"/>
       <c r="P95" t="inlineStr">
         <is>
           <t>https://www.nemokennislink.nl/publicaties/zie-ik-spoken/</t>
@@ -6379,11 +6187,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O97" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O97" t="inlineStr"/>
       <c r="P97" t="inlineStr">
         <is>
           <t>https://www.rivm.nl/burgerwetenschap/shift-diets</t>
@@ -6507,11 +6311,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O99" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O99" t="inlineStr"/>
       <c r="P99" t="inlineStr">
         <is>
           <t>https://www.rug.nl/sciencelinx/maatschappij/curious</t>
@@ -6573,11 +6373,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O100" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O100" t="inlineStr"/>
       <c r="P100" t="inlineStr">
         <is>
           <t>http://www.kijkeengezondewijk.nl/#/info</t>
@@ -6635,11 +6431,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O101" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O101" t="inlineStr"/>
       <c r="P101" t="inlineStr">
         <is>
           <t>https://www.iedereenwetenschapper.be/projects/hoe-snel-herken-jij-een-liedje</t>
@@ -6823,11 +6615,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O104" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O104" t="inlineStr"/>
       <c r="P104" t="inlineStr">
         <is>
           <t>https://ronaldbierings.com/over-zicht-op-licht/</t>
@@ -6883,11 +6671,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O105" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O105" t="inlineStr"/>
       <c r="P105" t="inlineStr">
         <is>
           <t>https://woordwaark.nl/stemmen/</t>
@@ -6943,11 +6727,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O106" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O106" t="inlineStr"/>
       <c r="P106" t="inlineStr">
         <is>
           <t>https://www.wetenschapsknooppunten.nl/alle-scholen-verzamelen/citizen-science/</t>
@@ -7003,11 +6783,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O107" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O107" t="inlineStr"/>
       <c r="P107" t="inlineStr">
         <is>
           <t>https://www.tudelft.nl/scd/waterlab/doe-mee-aan-onderzoek/project-6-nationale-plasticwatch</t>
@@ -7125,11 +6901,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O109" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O109" t="inlineStr"/>
       <c r="P109" t="inlineStr">
         <is>
           <t>https://www.zooniverse.org/projects/anneoverduin/fishing-in-the-past/about/research</t>
@@ -7375,11 +7147,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O113" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O113" t="inlineStr"/>
       <c r="P113" t="inlineStr">
         <is>
           <t>https://www.naturetoday.com/intl/nl/nature-reports/message/?msg=25068</t>
@@ -7439,11 +7207,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O114" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O114" t="inlineStr"/>
       <c r="P114" t="inlineStr">
         <is>
           <t>https://www.naturetoday.com/intl/nl/nature-reports/message/?msg=22655</t>
@@ -7925,11 +7689,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O122" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O122" t="inlineStr"/>
       <c r="P122" t="inlineStr">
         <is>
           <t>https://www.universiteitleiden.nl/citizensciencelab/projecten/evoscope---koolmezen</t>
@@ -8291,11 +8051,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O128" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O128" t="inlineStr"/>
       <c r="P128" t="inlineStr">
         <is>
           <t>https://www.floron.nl/meedoen/herbariummateriaal</t>
@@ -8415,11 +8171,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O130" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O130" t="inlineStr"/>
       <c r="P130" t="inlineStr">
         <is>
           <t>https://www.iedereenwetenschapper.be/projects/bestudeer-wilde-dieren-de-hoge-veluwe</t>
@@ -8535,11 +8287,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O132" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O132" t="inlineStr"/>
       <c r="P132" t="inlineStr">
         <is>
           <t>https://submit.cr-birding.org/page/who_are_we/</t>
@@ -8595,11 +8343,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O133" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O133" t="inlineStr"/>
       <c r="P133" t="inlineStr">
         <is>
           <t>https://www.naturetoday.com/intl/nl/nature-reports/message/?msg=27308</t>
@@ -8895,11 +8639,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O138" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O138" t="inlineStr"/>
       <c r="P138" t="inlineStr">
         <is>
           <t>https://www.naturetoday.com/intl/nl/nature-reports/message/?msg=26207</t>
@@ -9081,11 +8821,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O141" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O141" t="inlineStr"/>
       <c r="P141" t="inlineStr">
         <is>
           <t>https://www.universiteitleiden.nl/citizensciencelab/projecten/evoscope---kauwtjes</t>
@@ -9203,11 +8939,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O143" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O143" t="inlineStr"/>
       <c r="P143" t="inlineStr">
         <is>
           <t>https://www.universiteitleiden.nl/citizensciencelab/projecten/evoscope---paardenbloemen</t>
@@ -9505,11 +9237,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O148" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O148" t="inlineStr"/>
       <c r="P148" t="inlineStr">
         <is>
           <t>https://www.hortusleiden.nl/onderwijs/stoepplantjes-1</t>
@@ -9571,11 +9299,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O149" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O149" t="inlineStr"/>
       <c r="P149" t="inlineStr">
         <is>
           <t>https://www.universiteitleiden.nl/citizensciencelab/projecten/oeverplanten</t>
@@ -9875,11 +9599,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O154" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O154" t="inlineStr"/>
       <c r="P154" t="inlineStr">
         <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/projecten/treewifi</t>
@@ -9999,11 +9719,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O156" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O156" t="inlineStr"/>
       <c r="P156" t="inlineStr">
         <is>
           <t>https://www.iedereenwetenschapper.be/projects/hoe-gaat-het-met-de-wilde-eend</t>
@@ -10605,11 +10321,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O166" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O166" t="inlineStr"/>
       <c r="P166" t="inlineStr">
         <is>
           <t>https://www.universiteitleiden.nl/citizensciencelab/projecten/erfgoed-gezocht</t>
@@ -10671,11 +10383,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O167" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O167" t="inlineStr"/>
       <c r="P167" t="inlineStr">
         <is>
           <t>https://www.archeologieleeft.nl/archeosuccessen/erfgoed-gezocht/</t>
@@ -10731,11 +10439,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O168" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O168" t="inlineStr"/>
       <c r="P168" t="inlineStr">
         <is>
           <t>https://www.universiteitleiden.nl/nieuws/2020/04/erfgoed-gezocht-junior-kinderen-speuren-vanuit-huis-mee-met-archeologen</t>
@@ -10857,11 +10561,7 @@
           <t>Unsure</t>
         </is>
       </c>
-      <c r="O170" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O170" t="inlineStr"/>
       <c r="P170" t="inlineStr">
         <is>
           <t>https://boerenmetenwater.nl/aanleiding/</t>
@@ -11175,11 +10875,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O175" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O175" t="inlineStr"/>
       <c r="P175" t="inlineStr">
         <is>
           <t>https://www.tudelft.nl/scd/waterlab/doe-mee-aan-onderzoek/project-4-oeverwatch</t>
@@ -11613,11 +11309,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O182" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O182" t="inlineStr"/>
       <c r="P182" t="inlineStr">
         <is>
           <t>https://www.tudelft.nl/scd/waterlab/doe-mee-aan-onderzoek/project-2-check-de-stadsvergroening</t>
@@ -11743,11 +11435,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O184" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O184" t="inlineStr"/>
       <c r="P184" t="inlineStr">
         <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/aireas-eindhoven</t>
@@ -11807,11 +11495,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O185" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O185" t="inlineStr"/>
       <c r="P185" t="inlineStr">
         <is>
           <t>https://www.naturalis.nl/collectie/verborgen-vlinders-het-gestroomlijnd-zichtbaar-maken-van-papillotten</t>
@@ -11993,11 +11677,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O188" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O188" t="inlineStr"/>
       <c r="P188" t="inlineStr">
         <is>
           <t>https://www.kwrwater.nl/projecten/citizen-science-praktijkpilot-versheid-water/</t>
@@ -12117,11 +11797,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O190" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O190" t="inlineStr"/>
       <c r="P190" t="inlineStr">
         <is>
           <t>https://www.flevoland.nl/dossiers/waterlab-circulair-water</t>
@@ -12307,11 +11983,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O193" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O193" t="inlineStr"/>
       <c r="P193" t="inlineStr">
         <is>
           <t>https://www.scorewater.eu/#3cases</t>
@@ -12619,11 +12291,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O198" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O198" t="inlineStr"/>
       <c r="P198" t="inlineStr">
         <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/visibilis</t>
@@ -12685,11 +12353,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O199" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O199" t="inlineStr"/>
       <c r="P199" t="inlineStr">
         <is>
           <t>https://www.waterforum.net/officiele-start-waterlab-flevoland/</t>
@@ -12871,11 +12535,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O202" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O202" t="inlineStr"/>
       <c r="P202" t="inlineStr">
         <is>
           <t>https://globenederland.nl/onderzoeksprojecten/lichtmeting/</t>
@@ -13125,11 +12785,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O206" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O206" t="inlineStr"/>
       <c r="P206" t="inlineStr">
         <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/airsenseur</t>
@@ -13313,11 +12969,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O209" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O209" t="inlineStr"/>
       <c r="P209" t="inlineStr">
         <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/metingen-s-gravendijkwal-rotterdam</t>
@@ -13435,11 +13087,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O211" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O211" t="inlineStr"/>
       <c r="P211" t="inlineStr">
         <is>
           <t>https://www.samenmetenaanluchtkwaliteit.nl/ispex</t>
@@ -14265,11 +13913,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O224" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O224" t="inlineStr"/>
       <c r="P224" t="inlineStr">
         <is>
           <t>https://www.tudelft.nl/scd/waterlab/doe-mee-aan-onderzoek/project-5-zet-m-op-70</t>
@@ -14387,11 +14031,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O226" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O226" t="inlineStr"/>
       <c r="P226" t="inlineStr">
         <is>
           <t>https://www.nemokennislink.nl/publicaties/doe-mee-aan-de-grote-griepmeting/</t>
@@ -14447,11 +14087,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O227" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O227" t="inlineStr"/>
       <c r="P227" t="inlineStr">
         <is>
           <t>https://www.rivm.nl/rivm/kennis-en-kunde/strategisch-programma-rivm/spr-2015-2018/integrale-risicobeoordeling/ik-heb-nu-last-app</t>
@@ -14571,11 +14207,7 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="O229" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O229" t="inlineStr"/>
       <c r="P229" t="inlineStr">
         <is>
           <t>https://www.jagersvereniging.nl/downloads/bestuurdersdocumenten/telprotocol-zomerganzentelling/</t>
@@ -14753,11 +14385,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O232" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="O232" t="inlineStr"/>
       <c r="P232" t="inlineStr">
         <is>
           <t>https://www.mycardio.nl/</t>

</xml_diff>